<commit_message>
Module for AutoPulling data from DHIS2 added
</commit_message>
<xml_diff>
--- a/web/aca_mca.xlsx
+++ b/web/aca_mca.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\InternalSystem\web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A8C9DD-2B72-49F8-92F1-57D80DFFF772}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD9D2EC-27AA-4B71-B258-2141DCCC0745}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="iDTxC2zUd8tD0P4TUlQVHSkYofbeXAmA87f/LJe0hkyTzekk5ZQsTXzmEU1eyaeNYm2PoUzIg+wK8/0CL7JSFg==" workbookSaltValue="iwxpMS94jm35+J1eIh/WPg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="771" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -23,7 +23,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">ACA!$A$1:$Q$18</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">MCA!$A$1:$N$18</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -878,19 +878,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="4"/>
-      </left>
-      <right style="medium">
-        <color theme="4"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color theme="4"/>
       </left>
@@ -1023,6 +1010,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF4472C4"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF4472C4"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF4472C4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF4472C4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1090,9 +1092,6 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1108,9 +1107,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1126,13 +1125,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1142,22 +1141,22 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="5" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1182,6 +1181,87 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1215,85 +1295,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1317,21 +1331,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2558,7 +2558,7 @@
       <selection activeCell="F2" sqref="F2:H2"/>
       <selection pane="topRight" activeCell="F2" sqref="F2:H2"/>
       <selection pane="bottomLeft" activeCell="F2" sqref="F2:H2"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2584,161 +2584,161 @@
       <c r="A1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="54" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="53"/>
-      <c r="E1" s="54" t="s">
+      <c r="D1" s="52"/>
+      <c r="E1" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="53">
+      <c r="F1" s="52">
         <v>10</v>
       </c>
-      <c r="G1" s="54" t="s">
+      <c r="G1" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="82">
+      <c r="H1" s="70">
         <v>2019</v>
       </c>
-      <c r="I1" s="83"/>
-      <c r="J1" s="84" t="s">
+      <c r="I1" s="71"/>
+      <c r="J1" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="77" t="str">
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="64" t="str">
         <f>IF(COUNTIF(R20:R25,"&lt;&gt;0"),"Report Has Errors","Report is Correct")</f>
         <v>Report is Correct</v>
       </c>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64"/>
     </row>
     <row r="2" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="89" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="92" t="s">
+      <c r="B2" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="67" t="s">
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="68"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="67" t="s">
+      <c r="M2" s="55"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="P2" s="68"/>
-      <c r="Q2" s="69"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="56"/>
     </row>
     <row r="3" spans="1:17" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="87"/>
-      <c r="B3" s="90"/>
-      <c r="C3" s="55" t="s">
+      <c r="A3" s="75"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="55" t="s">
+      <c r="D3" s="82"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="56"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="55" t="s">
+      <c r="G3" s="82"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="56"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="70" t="s">
+      <c r="J3" s="82"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="M3" s="71"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="70" t="s">
+      <c r="M3" s="58"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="P3" s="71"/>
-      <c r="Q3" s="72"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="59"/>
     </row>
     <row r="4" spans="1:17" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="87"/>
-      <c r="B4" s="90"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="63"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="74"/>
-      <c r="N4" s="75"/>
-      <c r="O4" s="73"/>
-      <c r="P4" s="74"/>
-      <c r="Q4" s="75"/>
+      <c r="A4" s="75"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="60"/>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="62"/>
     </row>
     <row r="5" spans="1:17" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="88"/>
-      <c r="B5" s="91"/>
-      <c r="C5" s="23" t="s">
+      <c r="A5" s="76"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="H5" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="24" t="s">
+      <c r="J5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="25" t="s">
+      <c r="K5" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="23" t="s">
+      <c r="L5" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="M5" s="24" t="s">
+      <c r="M5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="25" t="s">
+      <c r="N5" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="O5" s="23" t="s">
+      <c r="O5" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="P5" s="24" t="s">
+      <c r="P5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="Q5" s="25" t="s">
+      <c r="Q5" s="24" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2751,16 +2751,28 @@
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
-      <c r="E6" s="22"/>
+      <c r="E6" s="3">
+        <f t="shared" ref="E6:E16" si="0">SUM(C6:D6)</f>
+        <v>0</v>
+      </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
-      <c r="H6" s="3"/>
+      <c r="H6" s="3">
+        <f t="shared" ref="H6:H16" si="1">SUM(F6:G6)</f>
+        <v>0</v>
+      </c>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
-      <c r="K6" s="3"/>
+      <c r="K6" s="3">
+        <f t="shared" ref="K6:K16" si="2">SUM(I6:J6)</f>
+        <v>0</v>
+      </c>
       <c r="L6" s="14"/>
       <c r="M6" s="14"/>
-      <c r="N6" s="3"/>
+      <c r="N6" s="3">
+        <f t="shared" ref="N6:N16" si="3">SUM(L6:M6)</f>
+        <v>0</v>
+      </c>
       <c r="O6" s="14"/>
       <c r="P6" s="14"/>
       <c r="Q6" s="3">
@@ -2778,25 +2790,25 @@
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="E7" s="3">
-        <f t="shared" ref="E7:E16" si="0">SUM(C7:D7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="3">
-        <f t="shared" ref="H7:H16" si="1">SUM(F7:G7)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
       <c r="K7" s="3">
-        <f t="shared" ref="K7:K16" si="2">SUM(I7:J7)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L7" s="13"/>
       <c r="M7" s="14"/>
       <c r="N7" s="3">
-        <f t="shared" ref="N7:N16" si="3">SUM(L7:M7)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O7" s="13"/>
@@ -3075,7 +3087,7 @@
         <f>C9-SUM(C10:C13)</f>
         <v>0</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="25">
         <f>D9-SUM(D10:D13)</f>
         <v>0</v>
       </c>
@@ -3083,11 +3095,11 @@
         <f t="shared" ref="E14:N14" si="8">E9-SUM(E10:E13)</f>
         <v>0</v>
       </c>
-      <c r="F14" s="26">
+      <c r="F14" s="25">
         <f>F9-SUM(F10:F13)</f>
         <v>0</v>
       </c>
-      <c r="G14" s="26">
+      <c r="G14" s="25">
         <f>G9-SUM(G10:G13)</f>
         <v>0</v>
       </c>
@@ -3095,11 +3107,11 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="I14" s="26">
+      <c r="I14" s="25">
         <f>I9-SUM(I10:I13)</f>
         <v>0</v>
       </c>
-      <c r="J14" s="26">
+      <c r="J14" s="25">
         <f>J9-SUM(J10:J13)</f>
         <v>0</v>
       </c>
@@ -3107,11 +3119,11 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="L14" s="26">
+      <c r="L14" s="25">
         <f>L9-SUM(L10:L13)</f>
         <v>0</v>
       </c>
-      <c r="M14" s="26">
+      <c r="M14" s="25">
         <f>M9-SUM(M10:M13)</f>
         <v>0</v>
       </c>
@@ -3119,11 +3131,11 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="O14" s="26">
+      <c r="O14" s="25">
         <f>O9-SUM(O10:O13)</f>
         <v>0</v>
       </c>
-      <c r="P14" s="26">
+      <c r="P14" s="25">
         <f>P9-SUM(P10:P13)</f>
         <v>0</v>
       </c>
@@ -3140,7 +3152,7 @@
         <v>23</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="26"/>
+      <c r="D15" s="25"/>
       <c r="E15" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3178,7 +3190,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="26"/>
+      <c r="D16" s="25"/>
       <c r="E16" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3277,1359 +3289,1365 @@
       </c>
     </row>
     <row r="18" spans="1:18" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="28" t="str">
+      <c r="C18" s="27" t="str">
         <f>IFERROR(C16/C15,"")</f>
         <v/>
       </c>
-      <c r="D18" s="29" t="str">
+      <c r="D18" s="28" t="str">
         <f t="shared" ref="D18:N18" si="13">IFERROR(D16/D15,"")</f>
         <v/>
       </c>
-      <c r="E18" s="30" t="str">
+      <c r="E18" s="29" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="F18" s="28" t="str">
+      <c r="F18" s="27" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="G18" s="29" t="str">
+      <c r="G18" s="28" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="H18" s="30" t="str">
+      <c r="H18" s="29" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="I18" s="28" t="str">
+      <c r="I18" s="27" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="J18" s="29" t="str">
+      <c r="J18" s="28" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="K18" s="30" t="str">
+      <c r="K18" s="29" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="L18" s="28" t="str">
+      <c r="L18" s="27" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="M18" s="29" t="str">
+      <c r="M18" s="28" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="N18" s="30" t="str">
+      <c r="N18" s="29" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="O18" s="28" t="str">
+      <c r="O18" s="27" t="str">
         <f t="shared" ref="O18:Q18" si="14">IFERROR(O16/O15,"")</f>
         <v/>
       </c>
-      <c r="P18" s="29" t="str">
+      <c r="P18" s="28" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="Q18" s="30" t="str">
+      <c r="Q18" s="29" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:18" ht="20.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="78" t="s">
+      <c r="A19" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="79"/>
-      <c r="C19" s="79"/>
-      <c r="D19" s="79"/>
-      <c r="E19" s="79"/>
-      <c r="F19" s="79"/>
-      <c r="G19" s="79"/>
-      <c r="H19" s="79"/>
-      <c r="I19" s="79"/>
-      <c r="J19" s="79"/>
-      <c r="K19" s="79"/>
-      <c r="L19" s="79"/>
-      <c r="M19" s="79"/>
-      <c r="N19" s="79"/>
-      <c r="O19" s="79"/>
-      <c r="P19" s="79"/>
-      <c r="Q19" s="80"/>
+      <c r="B19" s="66"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="66"/>
+      <c r="H19" s="66"/>
+      <c r="I19" s="66"/>
+      <c r="J19" s="66"/>
+      <c r="K19" s="66"/>
+      <c r="L19" s="66"/>
+      <c r="M19" s="66"/>
+      <c r="N19" s="66"/>
+      <c r="O19" s="66"/>
+      <c r="P19" s="66"/>
+      <c r="Q19" s="67"/>
     </row>
     <row r="20" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="66"/>
-      <c r="C20" s="50">
+      <c r="B20" s="68"/>
+      <c r="C20" s="49">
         <f>C14</f>
         <v>0</v>
       </c>
-      <c r="D20" s="50">
+      <c r="D20" s="49">
         <f>D14</f>
         <v>0</v>
       </c>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50">
+      <c r="E20" s="49"/>
+      <c r="F20" s="49">
         <f>F14</f>
         <v>0</v>
       </c>
-      <c r="G20" s="50">
+      <c r="G20" s="49">
         <f>G14</f>
         <v>0</v>
       </c>
-      <c r="H20" s="50"/>
-      <c r="I20" s="50">
+      <c r="H20" s="49"/>
+      <c r="I20" s="49">
         <f>I14</f>
         <v>0</v>
       </c>
-      <c r="J20" s="50">
+      <c r="J20" s="49">
         <f>J14</f>
         <v>0</v>
       </c>
-      <c r="K20" s="50"/>
-      <c r="L20" s="50">
+      <c r="K20" s="49"/>
+      <c r="L20" s="49">
         <f>L14</f>
         <v>0</v>
       </c>
-      <c r="M20" s="50">
+      <c r="M20" s="49">
         <f>M14</f>
         <v>0</v>
       </c>
-      <c r="N20" s="50"/>
-      <c r="O20" s="50">
+      <c r="N20" s="49"/>
+      <c r="O20" s="49">
         <f>O14</f>
         <v>0</v>
       </c>
-      <c r="P20" s="50">
+      <c r="P20" s="49">
         <f>P14</f>
         <v>0</v>
       </c>
-      <c r="Q20" s="50"/>
-      <c r="R20" s="27">
+      <c r="Q20" s="49"/>
+      <c r="R20" s="26">
         <f>COUNTIF(C20:Q20,"&lt;0")</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="66" t="s">
+      <c r="A21" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="66"/>
-      <c r="C21" s="50">
+      <c r="B21" s="68"/>
+      <c r="C21" s="49">
         <f>C15-C16</f>
         <v>0</v>
       </c>
-      <c r="D21" s="50">
+      <c r="D21" s="49">
         <f>D15-D16</f>
         <v>0</v>
       </c>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50">
+      <c r="E21" s="49"/>
+      <c r="F21" s="49">
         <f>F15-F16</f>
         <v>0</v>
       </c>
-      <c r="G21" s="50">
+      <c r="G21" s="49">
         <f>G15-G16</f>
         <v>0</v>
       </c>
-      <c r="H21" s="50"/>
-      <c r="I21" s="50">
+      <c r="H21" s="49"/>
+      <c r="I21" s="49">
         <f>I15-I16</f>
         <v>0</v>
       </c>
-      <c r="J21" s="50">
+      <c r="J21" s="49">
         <f>J15-J16</f>
         <v>0</v>
       </c>
-      <c r="K21" s="50"/>
-      <c r="L21" s="50">
+      <c r="K21" s="49"/>
+      <c r="L21" s="49">
         <f>L15-L16</f>
         <v>0</v>
       </c>
-      <c r="M21" s="50">
+      <c r="M21" s="49">
         <f>M15-M16</f>
         <v>0</v>
       </c>
-      <c r="N21" s="50"/>
-      <c r="O21" s="50">
+      <c r="N21" s="49"/>
+      <c r="O21" s="49">
         <f>O15-O16</f>
         <v>0</v>
       </c>
-      <c r="P21" s="50">
+      <c r="P21" s="49">
         <f>P15-P16</f>
         <v>0</v>
       </c>
-      <c r="Q21" s="50"/>
-      <c r="R21" s="50">
+      <c r="Q21" s="49"/>
+      <c r="R21" s="49">
         <f t="shared" ref="R21:R25" si="15">COUNTIF(C21:Q21,"&lt;0")</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="66"/>
-      <c r="C22" s="32" t="str">
+      <c r="B22" s="68"/>
+      <c r="C22" s="31" t="str">
         <f>IF(C20&lt;0,C$26&amp;"  Has "&amp;$A22,"")</f>
         <v/>
       </c>
-      <c r="D22" s="32" t="str">
+      <c r="D22" s="31" t="str">
         <f t="shared" ref="D22:N23" si="16">IF(D20&lt;0,D$26&amp;"  Has "&amp;$A22,"")</f>
         <v/>
       </c>
-      <c r="E22" s="32" t="str">
+      <c r="E22" s="31" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="F22" s="32" t="str">
+      <c r="F22" s="31" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="G22" s="32" t="str">
+      <c r="G22" s="31" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="H22" s="32" t="str">
+      <c r="H22" s="31" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="I22" s="32" t="str">
+      <c r="I22" s="31" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="J22" s="32" t="str">
+      <c r="J22" s="31" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="K22" s="32" t="str">
+      <c r="K22" s="31" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="L22" s="32" t="str">
+      <c r="L22" s="31" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="M22" s="32" t="str">
+      <c r="M22" s="31" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="N22" s="32" t="str">
+      <c r="N22" s="31" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="O22" s="32" t="str">
+      <c r="O22" s="31" t="str">
         <f t="shared" ref="O22:Q22" si="17">IF(O20&lt;0,O$26&amp;"  Has "&amp;$A22,"")</f>
         <v/>
       </c>
-      <c r="P22" s="32" t="str">
+      <c r="P22" s="31" t="str">
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="Q22" s="32" t="str">
+      <c r="Q22" s="31" t="str">
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="R22" s="50">
+      <c r="R22" s="49">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="81" t="s">
+      <c r="A23" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="81"/>
-      <c r="C23" s="32" t="str">
+      <c r="B23" s="69"/>
+      <c r="C23" s="31" t="str">
         <f>IF(C21&lt;0,C$26&amp;"  Has "&amp;$A23,"")</f>
         <v/>
       </c>
-      <c r="D23" s="32" t="str">
+      <c r="D23" s="31" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="E23" s="32" t="str">
+      <c r="E23" s="31" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="F23" s="32" t="str">
+      <c r="F23" s="31" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="G23" s="32" t="str">
+      <c r="G23" s="31" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="H23" s="32" t="str">
+      <c r="H23" s="31" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="I23" s="32" t="str">
+      <c r="I23" s="31" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="J23" s="32" t="str">
+      <c r="J23" s="31" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="K23" s="32" t="str">
+      <c r="K23" s="31" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="L23" s="32" t="str">
+      <c r="L23" s="31" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="M23" s="32" t="str">
+      <c r="M23" s="31" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="N23" s="32" t="str">
+      <c r="N23" s="31" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="O23" s="32" t="str">
+      <c r="O23" s="31" t="str">
         <f t="shared" ref="O23:Q23" si="18">IF(O21&lt;0,O$26&amp;"  Has "&amp;$A23,"")</f>
         <v/>
       </c>
-      <c r="P23" s="32" t="str">
+      <c r="P23" s="31" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="Q23" s="32" t="str">
+      <c r="Q23" s="31" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="R23" s="50">
+      <c r="R23" s="49">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="65" t="s">
+      <c r="A24" s="91" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="65"/>
-      <c r="C24" s="52">
-        <f>C6-F6-I6</f>
-        <v>0</v>
-      </c>
-      <c r="D24" s="52">
-        <f>D6-G6-J6</f>
-        <v>0</v>
-      </c>
-      <c r="E24" s="52">
+      <c r="B24" s="91"/>
+      <c r="C24" s="51">
+        <f>(C6-F6)-(F6-I6)</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="51">
+        <f>(D6-G6)-(G6-J6)</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="51">
         <f>IF(C24&lt;&gt;0,-1,IF(D24&lt;&gt;0,-1,0))</f>
         <v>0</v>
       </c>
-      <c r="F24" s="52"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="52"/>
-      <c r="L24" s="52"/>
-      <c r="M24" s="52"/>
-      <c r="N24" s="52"/>
-      <c r="O24" s="52"/>
-      <c r="P24" s="52"/>
-      <c r="Q24" s="52"/>
-      <c r="R24" s="50">
+      <c r="F24" s="51"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="51"/>
+      <c r="L24" s="51"/>
+      <c r="M24" s="51"/>
+      <c r="N24" s="51"/>
+      <c r="O24" s="51"/>
+      <c r="P24" s="51"/>
+      <c r="Q24" s="51"/>
+      <c r="R24" s="49">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="66" t="s">
+      <c r="A25" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="66"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="52">
+      <c r="B25" s="68"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51">
         <f>F14-F15</f>
         <v>0</v>
       </c>
-      <c r="G25" s="52">
+      <c r="G25" s="51">
         <f>G14-G15</f>
         <v>0</v>
       </c>
-      <c r="H25" s="52"/>
-      <c r="I25" s="52">
+      <c r="H25" s="51"/>
+      <c r="I25" s="51">
         <f>I14-I15</f>
         <v>0</v>
       </c>
-      <c r="J25" s="52">
+      <c r="J25" s="51">
         <f>J14-J15</f>
         <v>0</v>
       </c>
-      <c r="K25" s="52"/>
-      <c r="L25" s="52">
+      <c r="K25" s="51"/>
+      <c r="L25" s="51">
         <f>L14-L15</f>
         <v>0</v>
       </c>
-      <c r="M25" s="52">
+      <c r="M25" s="51">
         <f>M14-M15</f>
         <v>0</v>
       </c>
-      <c r="N25" s="52"/>
-      <c r="O25" s="52">
+      <c r="N25" s="51"/>
+      <c r="O25" s="51">
         <f>O14-O15</f>
         <v>0</v>
       </c>
-      <c r="P25" s="52">
+      <c r="P25" s="51">
         <f>P14-P15</f>
         <v>0</v>
       </c>
-      <c r="Q25" s="52"/>
-      <c r="R25" s="50">
+      <c r="Q25" s="51"/>
+      <c r="R25" s="49">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="64" t="s">
+      <c r="A26" s="90" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="64"/>
-      <c r="C26" s="51" t="str">
+      <c r="B26" s="90"/>
+      <c r="C26" s="50" t="str">
         <f>$C3&amp;" "&amp;C5</f>
         <v>3 months cohort Adults</v>
       </c>
-      <c r="D26" s="51" t="str">
+      <c r="D26" s="50" t="str">
         <f>$C3&amp;" "&amp;D5</f>
         <v>3 months cohort children</v>
       </c>
-      <c r="E26" s="51" t="str">
+      <c r="E26" s="50" t="str">
         <f>$C3&amp;" "&amp;E5</f>
         <v>3 months cohort Total</v>
       </c>
-      <c r="F26" s="51" t="str">
+      <c r="F26" s="50" t="str">
         <f>$F3&amp;" "&amp;F5</f>
         <v>6 months cohort Adults</v>
       </c>
-      <c r="G26" s="51" t="str">
+      <c r="G26" s="50" t="str">
         <f>$F3&amp;" "&amp;G5</f>
         <v>6 months cohort children</v>
       </c>
-      <c r="H26" s="51" t="str">
+      <c r="H26" s="50" t="str">
         <f>$F3&amp;" "&amp;H5</f>
         <v>6 months cohort Total</v>
       </c>
-      <c r="I26" s="51" t="str">
+      <c r="I26" s="50" t="str">
         <f>$I3&amp;" "&amp;I5</f>
         <v>12 months cohort Adults</v>
       </c>
-      <c r="J26" s="51" t="str">
+      <c r="J26" s="50" t="str">
         <f t="shared" ref="J26:K26" si="19">$I3&amp;" "&amp;J5</f>
         <v>12 months cohort children</v>
       </c>
-      <c r="K26" s="51" t="str">
+      <c r="K26" s="50" t="str">
         <f t="shared" si="19"/>
         <v>12 months cohort Total</v>
       </c>
-      <c r="L26" s="51" t="str">
+      <c r="L26" s="50" t="str">
         <f>$L3&amp;" "&amp;L5</f>
         <v>24 months cohort Adults</v>
       </c>
-      <c r="M26" s="51" t="str">
+      <c r="M26" s="50" t="str">
         <f>$L3&amp;" "&amp;M5</f>
         <v>24 months cohort children</v>
       </c>
-      <c r="N26" s="51" t="str">
+      <c r="N26" s="50" t="str">
         <f>$L3&amp;" "&amp;N5</f>
         <v>24 months cohort Total</v>
       </c>
-      <c r="O26" s="51" t="str">
+      <c r="O26" s="50" t="str">
         <f>$O3&amp;" "&amp;O5</f>
         <v>36 months cohort Adults</v>
       </c>
-      <c r="P26" s="51" t="str">
+      <c r="P26" s="50" t="str">
         <f t="shared" ref="P26:Q26" si="20">$O3&amp;" "&amp;P5</f>
         <v>36 months cohort children</v>
       </c>
-      <c r="Q26" s="51" t="str">
+      <c r="Q26" s="50" t="str">
         <f t="shared" si="20"/>
         <v>36 months cohort Total</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="76" t="str">
+      <c r="A28" s="63" t="str">
         <f>C22&amp;CHAR(10) &amp;D22 &amp;CHAR(10) &amp;E22 &amp;CHAR(10) &amp;F22 &amp; CHAR( 10 ) &amp;G22 &amp; CHAR( 10 ) &amp;H22 &amp; CHAR( 10 ) &amp;I22 &amp; CHAR( 10 ) &amp;J22 &amp; CHAR( 10 ) &amp;K22 &amp; CHAR( 10 ) &amp;L22 &amp; CHAR( 10 ) &amp;M22 &amp; CHAR( 10 ) &amp;N22 &amp; CHAR( 10 ) &amp;C23 &amp; CHAR( 10 ) &amp;D23 &amp; CHAR( 10 ) &amp;E23 &amp; CHAR( 10 ) &amp;F23 &amp; CHAR( 10 ) &amp;G23 &amp; CHAR( 10 ) &amp;H23 &amp; CHAR( 10 ) &amp;I23 &amp; CHAR( 10 ) &amp;J23 &amp; CHAR( 10 ) &amp;K23 &amp; CHAR( 10 ) &amp;L23 &amp; CHAR( 10 ) &amp;M23 &amp; CHAR( 10 ) &amp;N23 &amp; CHAR( 10 ) &amp;O22 &amp; CHAR( 10 ) &amp;P22 &amp; CHAR( 10 ) &amp;Q22 &amp; CHAR( 10 ) &amp;O23 &amp; CHAR( 10 ) &amp;P23 &amp; CHAR( 10 ) &amp;Q23</f>
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="B28" s="76"/>
-      <c r="C28" s="76"/>
-      <c r="D28" s="76"/>
-      <c r="E28" s="76"/>
-      <c r="F28" s="76"/>
-      <c r="G28" s="76"/>
-      <c r="H28" s="76"/>
-      <c r="I28" s="76"/>
-      <c r="J28" s="76"/>
-      <c r="K28" s="76"/>
-      <c r="L28" s="76"/>
-      <c r="M28" s="76"/>
-      <c r="N28" s="76"/>
-      <c r="O28" s="76"/>
-      <c r="P28" s="76"/>
-      <c r="Q28" s="76"/>
+      <c r="B28" s="63"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="63"/>
+      <c r="G28" s="63"/>
+      <c r="H28" s="63"/>
+      <c r="I28" s="63"/>
+      <c r="J28" s="63"/>
+      <c r="K28" s="63"/>
+      <c r="L28" s="63"/>
+      <c r="M28" s="63"/>
+      <c r="N28" s="63"/>
+      <c r="O28" s="63"/>
+      <c r="P28" s="63"/>
+      <c r="Q28" s="63"/>
     </row>
     <row r="29" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="76"/>
-      <c r="B29" s="76"/>
-      <c r="C29" s="76"/>
-      <c r="D29" s="76"/>
-      <c r="E29" s="76"/>
-      <c r="F29" s="76"/>
-      <c r="G29" s="76"/>
-      <c r="H29" s="76"/>
-      <c r="I29" s="76"/>
-      <c r="J29" s="76"/>
-      <c r="K29" s="76"/>
-      <c r="L29" s="76"/>
-      <c r="M29" s="76"/>
-      <c r="N29" s="76"/>
-      <c r="O29" s="76"/>
-      <c r="P29" s="76"/>
-      <c r="Q29" s="76"/>
+      <c r="A29" s="63"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="63"/>
+      <c r="H29" s="63"/>
+      <c r="I29" s="63"/>
+      <c r="J29" s="63"/>
+      <c r="K29" s="63"/>
+      <c r="L29" s="63"/>
+      <c r="M29" s="63"/>
+      <c r="N29" s="63"/>
+      <c r="O29" s="63"/>
+      <c r="P29" s="63"/>
+      <c r="Q29" s="63"/>
     </row>
     <row r="30" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="76"/>
-      <c r="B30" s="76"/>
-      <c r="C30" s="76"/>
-      <c r="D30" s="76"/>
-      <c r="E30" s="76"/>
-      <c r="F30" s="76"/>
-      <c r="G30" s="76"/>
-      <c r="H30" s="76"/>
-      <c r="I30" s="76"/>
-      <c r="J30" s="76"/>
-      <c r="K30" s="76"/>
-      <c r="L30" s="76"/>
-      <c r="M30" s="76"/>
-      <c r="N30" s="76"/>
-      <c r="O30" s="76"/>
-      <c r="P30" s="76"/>
-      <c r="Q30" s="76"/>
+      <c r="A30" s="63"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="63"/>
+      <c r="F30" s="63"/>
+      <c r="G30" s="63"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="63"/>
+      <c r="J30" s="63"/>
+      <c r="K30" s="63"/>
+      <c r="L30" s="63"/>
+      <c r="M30" s="63"/>
+      <c r="N30" s="63"/>
+      <c r="O30" s="63"/>
+      <c r="P30" s="63"/>
+      <c r="Q30" s="63"/>
     </row>
     <row r="31" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="76"/>
-      <c r="B31" s="76"/>
-      <c r="C31" s="76"/>
-      <c r="D31" s="76"/>
-      <c r="E31" s="76"/>
-      <c r="F31" s="76"/>
-      <c r="G31" s="76"/>
-      <c r="H31" s="76"/>
-      <c r="I31" s="76"/>
-      <c r="J31" s="76"/>
-      <c r="K31" s="76"/>
-      <c r="L31" s="76"/>
-      <c r="M31" s="76"/>
-      <c r="N31" s="76"/>
-      <c r="O31" s="76"/>
-      <c r="P31" s="76"/>
-      <c r="Q31" s="76"/>
+      <c r="A31" s="63"/>
+      <c r="B31" s="63"/>
+      <c r="C31" s="63"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="63"/>
+      <c r="G31" s="63"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="63"/>
+      <c r="J31" s="63"/>
+      <c r="K31" s="63"/>
+      <c r="L31" s="63"/>
+      <c r="M31" s="63"/>
+      <c r="N31" s="63"/>
+      <c r="O31" s="63"/>
+      <c r="P31" s="63"/>
+      <c r="Q31" s="63"/>
     </row>
     <row r="32" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="76"/>
-      <c r="B32" s="76"/>
-      <c r="C32" s="76"/>
-      <c r="D32" s="76"/>
-      <c r="E32" s="76"/>
-      <c r="F32" s="76"/>
-      <c r="G32" s="76"/>
-      <c r="H32" s="76"/>
-      <c r="I32" s="76"/>
-      <c r="J32" s="76"/>
-      <c r="K32" s="76"/>
-      <c r="L32" s="76"/>
-      <c r="M32" s="76"/>
-      <c r="N32" s="76"/>
-      <c r="O32" s="76"/>
-      <c r="P32" s="76"/>
-      <c r="Q32" s="76"/>
+      <c r="A32" s="63"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="63"/>
+      <c r="M32" s="63"/>
+      <c r="N32" s="63"/>
+      <c r="O32" s="63"/>
+      <c r="P32" s="63"/>
+      <c r="Q32" s="63"/>
     </row>
     <row r="33" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="76"/>
-      <c r="B33" s="76"/>
-      <c r="C33" s="76"/>
-      <c r="D33" s="76"/>
-      <c r="E33" s="76"/>
-      <c r="F33" s="76"/>
-      <c r="G33" s="76"/>
-      <c r="H33" s="76"/>
-      <c r="I33" s="76"/>
-      <c r="J33" s="76"/>
-      <c r="K33" s="76"/>
-      <c r="L33" s="76"/>
-      <c r="M33" s="76"/>
-      <c r="N33" s="76"/>
-      <c r="O33" s="76"/>
-      <c r="P33" s="76"/>
-      <c r="Q33" s="76"/>
+      <c r="A33" s="63"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="63"/>
+      <c r="K33" s="63"/>
+      <c r="L33" s="63"/>
+      <c r="M33" s="63"/>
+      <c r="N33" s="63"/>
+      <c r="O33" s="63"/>
+      <c r="P33" s="63"/>
+      <c r="Q33" s="63"/>
     </row>
     <row r="34" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="76"/>
-      <c r="B34" s="76"/>
-      <c r="C34" s="76"/>
-      <c r="D34" s="76"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="76"/>
-      <c r="G34" s="76"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="76"/>
-      <c r="J34" s="76"/>
-      <c r="K34" s="76"/>
-      <c r="L34" s="76"/>
-      <c r="M34" s="76"/>
-      <c r="N34" s="76"/>
-      <c r="O34" s="76"/>
-      <c r="P34" s="76"/>
-      <c r="Q34" s="76"/>
+      <c r="A34" s="63"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="63"/>
+      <c r="G34" s="63"/>
+      <c r="H34" s="63"/>
+      <c r="I34" s="63"/>
+      <c r="J34" s="63"/>
+      <c r="K34" s="63"/>
+      <c r="L34" s="63"/>
+      <c r="M34" s="63"/>
+      <c r="N34" s="63"/>
+      <c r="O34" s="63"/>
+      <c r="P34" s="63"/>
+      <c r="Q34" s="63"/>
     </row>
     <row r="35" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="76"/>
-      <c r="B35" s="76"/>
-      <c r="C35" s="76"/>
-      <c r="D35" s="76"/>
-      <c r="E35" s="76"/>
-      <c r="F35" s="76"/>
-      <c r="G35" s="76"/>
-      <c r="H35" s="76"/>
-      <c r="I35" s="76"/>
-      <c r="J35" s="76"/>
-      <c r="K35" s="76"/>
-      <c r="L35" s="76"/>
-      <c r="M35" s="76"/>
-      <c r="N35" s="76"/>
-      <c r="O35" s="76"/>
-      <c r="P35" s="76"/>
-      <c r="Q35" s="76"/>
+      <c r="A35" s="63"/>
+      <c r="B35" s="63"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="63"/>
+      <c r="G35" s="63"/>
+      <c r="H35" s="63"/>
+      <c r="I35" s="63"/>
+      <c r="J35" s="63"/>
+      <c r="K35" s="63"/>
+      <c r="L35" s="63"/>
+      <c r="M35" s="63"/>
+      <c r="N35" s="63"/>
+      <c r="O35" s="63"/>
+      <c r="P35" s="63"/>
+      <c r="Q35" s="63"/>
     </row>
     <row r="36" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="76"/>
-      <c r="B36" s="76"/>
-      <c r="C36" s="76"/>
-      <c r="D36" s="76"/>
-      <c r="E36" s="76"/>
-      <c r="F36" s="76"/>
-      <c r="G36" s="76"/>
-      <c r="H36" s="76"/>
-      <c r="I36" s="76"/>
-      <c r="J36" s="76"/>
-      <c r="K36" s="76"/>
-      <c r="L36" s="76"/>
-      <c r="M36" s="76"/>
-      <c r="N36" s="76"/>
-      <c r="O36" s="76"/>
-      <c r="P36" s="76"/>
-      <c r="Q36" s="76"/>
+      <c r="A36" s="63"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="63"/>
+      <c r="E36" s="63"/>
+      <c r="F36" s="63"/>
+      <c r="G36" s="63"/>
+      <c r="H36" s="63"/>
+      <c r="I36" s="63"/>
+      <c r="J36" s="63"/>
+      <c r="K36" s="63"/>
+      <c r="L36" s="63"/>
+      <c r="M36" s="63"/>
+      <c r="N36" s="63"/>
+      <c r="O36" s="63"/>
+      <c r="P36" s="63"/>
+      <c r="Q36" s="63"/>
     </row>
     <row r="37" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="76"/>
-      <c r="B37" s="76"/>
-      <c r="C37" s="76"/>
-      <c r="D37" s="76"/>
-      <c r="E37" s="76"/>
-      <c r="F37" s="76"/>
-      <c r="G37" s="76"/>
-      <c r="H37" s="76"/>
-      <c r="I37" s="76"/>
-      <c r="J37" s="76"/>
-      <c r="K37" s="76"/>
-      <c r="L37" s="76"/>
-      <c r="M37" s="76"/>
-      <c r="N37" s="76"/>
-      <c r="O37" s="76"/>
-      <c r="P37" s="76"/>
-      <c r="Q37" s="76"/>
+      <c r="A37" s="63"/>
+      <c r="B37" s="63"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="63"/>
+      <c r="F37" s="63"/>
+      <c r="G37" s="63"/>
+      <c r="H37" s="63"/>
+      <c r="I37" s="63"/>
+      <c r="J37" s="63"/>
+      <c r="K37" s="63"/>
+      <c r="L37" s="63"/>
+      <c r="M37" s="63"/>
+      <c r="N37" s="63"/>
+      <c r="O37" s="63"/>
+      <c r="P37" s="63"/>
+      <c r="Q37" s="63"/>
     </row>
     <row r="38" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="76"/>
-      <c r="B38" s="76"/>
-      <c r="C38" s="76"/>
-      <c r="D38" s="76"/>
-      <c r="E38" s="76"/>
-      <c r="F38" s="76"/>
-      <c r="G38" s="76"/>
-      <c r="H38" s="76"/>
-      <c r="I38" s="76"/>
-      <c r="J38" s="76"/>
-      <c r="K38" s="76"/>
-      <c r="L38" s="76"/>
-      <c r="M38" s="76"/>
-      <c r="N38" s="76"/>
-      <c r="O38" s="76"/>
-      <c r="P38" s="76"/>
-      <c r="Q38" s="76"/>
+      <c r="A38" s="63"/>
+      <c r="B38" s="63"/>
+      <c r="C38" s="63"/>
+      <c r="D38" s="63"/>
+      <c r="E38" s="63"/>
+      <c r="F38" s="63"/>
+      <c r="G38" s="63"/>
+      <c r="H38" s="63"/>
+      <c r="I38" s="63"/>
+      <c r="J38" s="63"/>
+      <c r="K38" s="63"/>
+      <c r="L38" s="63"/>
+      <c r="M38" s="63"/>
+      <c r="N38" s="63"/>
+      <c r="O38" s="63"/>
+      <c r="P38" s="63"/>
+      <c r="Q38" s="63"/>
     </row>
     <row r="39" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="76"/>
-      <c r="B39" s="76"/>
-      <c r="C39" s="76"/>
-      <c r="D39" s="76"/>
-      <c r="E39" s="76"/>
-      <c r="F39" s="76"/>
-      <c r="G39" s="76"/>
-      <c r="H39" s="76"/>
-      <c r="I39" s="76"/>
-      <c r="J39" s="76"/>
-      <c r="K39" s="76"/>
-      <c r="L39" s="76"/>
-      <c r="M39" s="76"/>
-      <c r="N39" s="76"/>
-      <c r="O39" s="76"/>
-      <c r="P39" s="76"/>
-      <c r="Q39" s="76"/>
+      <c r="A39" s="63"/>
+      <c r="B39" s="63"/>
+      <c r="C39" s="63"/>
+      <c r="D39" s="63"/>
+      <c r="E39" s="63"/>
+      <c r="F39" s="63"/>
+      <c r="G39" s="63"/>
+      <c r="H39" s="63"/>
+      <c r="I39" s="63"/>
+      <c r="J39" s="63"/>
+      <c r="K39" s="63"/>
+      <c r="L39" s="63"/>
+      <c r="M39" s="63"/>
+      <c r="N39" s="63"/>
+      <c r="O39" s="63"/>
+      <c r="P39" s="63"/>
+      <c r="Q39" s="63"/>
     </row>
     <row r="40" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="76"/>
-      <c r="B40" s="76"/>
-      <c r="C40" s="76"/>
-      <c r="D40" s="76"/>
-      <c r="E40" s="76"/>
-      <c r="F40" s="76"/>
-      <c r="G40" s="76"/>
-      <c r="H40" s="76"/>
-      <c r="I40" s="76"/>
-      <c r="J40" s="76"/>
-      <c r="K40" s="76"/>
-      <c r="L40" s="76"/>
-      <c r="M40" s="76"/>
-      <c r="N40" s="76"/>
-      <c r="O40" s="76"/>
-      <c r="P40" s="76"/>
-      <c r="Q40" s="76"/>
+      <c r="A40" s="63"/>
+      <c r="B40" s="63"/>
+      <c r="C40" s="63"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="63"/>
+      <c r="F40" s="63"/>
+      <c r="G40" s="63"/>
+      <c r="H40" s="63"/>
+      <c r="I40" s="63"/>
+      <c r="J40" s="63"/>
+      <c r="K40" s="63"/>
+      <c r="L40" s="63"/>
+      <c r="M40" s="63"/>
+      <c r="N40" s="63"/>
+      <c r="O40" s="63"/>
+      <c r="P40" s="63"/>
+      <c r="Q40" s="63"/>
     </row>
     <row r="41" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="76"/>
-      <c r="B41" s="76"/>
-      <c r="C41" s="76"/>
-      <c r="D41" s="76"/>
-      <c r="E41" s="76"/>
-      <c r="F41" s="76"/>
-      <c r="G41" s="76"/>
-      <c r="H41" s="76"/>
-      <c r="I41" s="76"/>
-      <c r="J41" s="76"/>
-      <c r="K41" s="76"/>
-      <c r="L41" s="76"/>
-      <c r="M41" s="76"/>
-      <c r="N41" s="76"/>
-      <c r="O41" s="76"/>
-      <c r="P41" s="76"/>
-      <c r="Q41" s="76"/>
+      <c r="A41" s="63"/>
+      <c r="B41" s="63"/>
+      <c r="C41" s="63"/>
+      <c r="D41" s="63"/>
+      <c r="E41" s="63"/>
+      <c r="F41" s="63"/>
+      <c r="G41" s="63"/>
+      <c r="H41" s="63"/>
+      <c r="I41" s="63"/>
+      <c r="J41" s="63"/>
+      <c r="K41" s="63"/>
+      <c r="L41" s="63"/>
+      <c r="M41" s="63"/>
+      <c r="N41" s="63"/>
+      <c r="O41" s="63"/>
+      <c r="P41" s="63"/>
+      <c r="Q41" s="63"/>
     </row>
     <row r="42" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="76"/>
-      <c r="B42" s="76"/>
-      <c r="C42" s="76"/>
-      <c r="D42" s="76"/>
-      <c r="E42" s="76"/>
-      <c r="F42" s="76"/>
-      <c r="G42" s="76"/>
-      <c r="H42" s="76"/>
-      <c r="I42" s="76"/>
-      <c r="J42" s="76"/>
-      <c r="K42" s="76"/>
-      <c r="L42" s="76"/>
-      <c r="M42" s="76"/>
-      <c r="N42" s="76"/>
-      <c r="O42" s="76"/>
-      <c r="P42" s="76"/>
-      <c r="Q42" s="76"/>
+      <c r="A42" s="63"/>
+      <c r="B42" s="63"/>
+      <c r="C42" s="63"/>
+      <c r="D42" s="63"/>
+      <c r="E42" s="63"/>
+      <c r="F42" s="63"/>
+      <c r="G42" s="63"/>
+      <c r="H42" s="63"/>
+      <c r="I42" s="63"/>
+      <c r="J42" s="63"/>
+      <c r="K42" s="63"/>
+      <c r="L42" s="63"/>
+      <c r="M42" s="63"/>
+      <c r="N42" s="63"/>
+      <c r="O42" s="63"/>
+      <c r="P42" s="63"/>
+      <c r="Q42" s="63"/>
     </row>
     <row r="43" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="76"/>
-      <c r="B43" s="76"/>
-      <c r="C43" s="76"/>
-      <c r="D43" s="76"/>
-      <c r="E43" s="76"/>
-      <c r="F43" s="76"/>
-      <c r="G43" s="76"/>
-      <c r="H43" s="76"/>
-      <c r="I43" s="76"/>
-      <c r="J43" s="76"/>
-      <c r="K43" s="76"/>
-      <c r="L43" s="76"/>
-      <c r="M43" s="76"/>
-      <c r="N43" s="76"/>
-      <c r="O43" s="76"/>
-      <c r="P43" s="76"/>
-      <c r="Q43" s="76"/>
+      <c r="A43" s="63"/>
+      <c r="B43" s="63"/>
+      <c r="C43" s="63"/>
+      <c r="D43" s="63"/>
+      <c r="E43" s="63"/>
+      <c r="F43" s="63"/>
+      <c r="G43" s="63"/>
+      <c r="H43" s="63"/>
+      <c r="I43" s="63"/>
+      <c r="J43" s="63"/>
+      <c r="K43" s="63"/>
+      <c r="L43" s="63"/>
+      <c r="M43" s="63"/>
+      <c r="N43" s="63"/>
+      <c r="O43" s="63"/>
+      <c r="P43" s="63"/>
+      <c r="Q43" s="63"/>
     </row>
     <row r="44" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="76"/>
-      <c r="B44" s="76"/>
-      <c r="C44" s="76"/>
-      <c r="D44" s="76"/>
-      <c r="E44" s="76"/>
-      <c r="F44" s="76"/>
-      <c r="G44" s="76"/>
-      <c r="H44" s="76"/>
-      <c r="I44" s="76"/>
-      <c r="J44" s="76"/>
-      <c r="K44" s="76"/>
-      <c r="L44" s="76"/>
-      <c r="M44" s="76"/>
-      <c r="N44" s="76"/>
-      <c r="O44" s="76"/>
-      <c r="P44" s="76"/>
-      <c r="Q44" s="76"/>
+      <c r="A44" s="63"/>
+      <c r="B44" s="63"/>
+      <c r="C44" s="63"/>
+      <c r="D44" s="63"/>
+      <c r="E44" s="63"/>
+      <c r="F44" s="63"/>
+      <c r="G44" s="63"/>
+      <c r="H44" s="63"/>
+      <c r="I44" s="63"/>
+      <c r="J44" s="63"/>
+      <c r="K44" s="63"/>
+      <c r="L44" s="63"/>
+      <c r="M44" s="63"/>
+      <c r="N44" s="63"/>
+      <c r="O44" s="63"/>
+      <c r="P44" s="63"/>
+      <c r="Q44" s="63"/>
     </row>
     <row r="45" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="76"/>
-      <c r="B45" s="76"/>
-      <c r="C45" s="76"/>
-      <c r="D45" s="76"/>
-      <c r="E45" s="76"/>
-      <c r="F45" s="76"/>
-      <c r="G45" s="76"/>
-      <c r="H45" s="76"/>
-      <c r="I45" s="76"/>
-      <c r="J45" s="76"/>
-      <c r="K45" s="76"/>
-      <c r="L45" s="76"/>
-      <c r="M45" s="76"/>
-      <c r="N45" s="76"/>
-      <c r="O45" s="76"/>
-      <c r="P45" s="76"/>
-      <c r="Q45" s="76"/>
+      <c r="A45" s="63"/>
+      <c r="B45" s="63"/>
+      <c r="C45" s="63"/>
+      <c r="D45" s="63"/>
+      <c r="E45" s="63"/>
+      <c r="F45" s="63"/>
+      <c r="G45" s="63"/>
+      <c r="H45" s="63"/>
+      <c r="I45" s="63"/>
+      <c r="J45" s="63"/>
+      <c r="K45" s="63"/>
+      <c r="L45" s="63"/>
+      <c r="M45" s="63"/>
+      <c r="N45" s="63"/>
+      <c r="O45" s="63"/>
+      <c r="P45" s="63"/>
+      <c r="Q45" s="63"/>
     </row>
     <row r="46" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="76"/>
-      <c r="B46" s="76"/>
-      <c r="C46" s="76"/>
-      <c r="D46" s="76"/>
-      <c r="E46" s="76"/>
-      <c r="F46" s="76"/>
-      <c r="G46" s="76"/>
-      <c r="H46" s="76"/>
-      <c r="I46" s="76"/>
-      <c r="J46" s="76"/>
-      <c r="K46" s="76"/>
-      <c r="L46" s="76"/>
-      <c r="M46" s="76"/>
-      <c r="N46" s="76"/>
-      <c r="O46" s="76"/>
-      <c r="P46" s="76"/>
-      <c r="Q46" s="76"/>
+      <c r="A46" s="63"/>
+      <c r="B46" s="63"/>
+      <c r="C46" s="63"/>
+      <c r="D46" s="63"/>
+      <c r="E46" s="63"/>
+      <c r="F46" s="63"/>
+      <c r="G46" s="63"/>
+      <c r="H46" s="63"/>
+      <c r="I46" s="63"/>
+      <c r="J46" s="63"/>
+      <c r="K46" s="63"/>
+      <c r="L46" s="63"/>
+      <c r="M46" s="63"/>
+      <c r="N46" s="63"/>
+      <c r="O46" s="63"/>
+      <c r="P46" s="63"/>
+      <c r="Q46" s="63"/>
     </row>
     <row r="47" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="76"/>
-      <c r="B47" s="76"/>
-      <c r="C47" s="76"/>
-      <c r="D47" s="76"/>
-      <c r="E47" s="76"/>
-      <c r="F47" s="76"/>
-      <c r="G47" s="76"/>
-      <c r="H47" s="76"/>
-      <c r="I47" s="76"/>
-      <c r="J47" s="76"/>
-      <c r="K47" s="76"/>
-      <c r="L47" s="76"/>
-      <c r="M47" s="76"/>
-      <c r="N47" s="76"/>
-      <c r="O47" s="76"/>
-      <c r="P47" s="76"/>
-      <c r="Q47" s="76"/>
+      <c r="A47" s="63"/>
+      <c r="B47" s="63"/>
+      <c r="C47" s="63"/>
+      <c r="D47" s="63"/>
+      <c r="E47" s="63"/>
+      <c r="F47" s="63"/>
+      <c r="G47" s="63"/>
+      <c r="H47" s="63"/>
+      <c r="I47" s="63"/>
+      <c r="J47" s="63"/>
+      <c r="K47" s="63"/>
+      <c r="L47" s="63"/>
+      <c r="M47" s="63"/>
+      <c r="N47" s="63"/>
+      <c r="O47" s="63"/>
+      <c r="P47" s="63"/>
+      <c r="Q47" s="63"/>
     </row>
     <row r="48" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="76"/>
-      <c r="B48" s="76"/>
-      <c r="C48" s="76"/>
-      <c r="D48" s="76"/>
-      <c r="E48" s="76"/>
-      <c r="F48" s="76"/>
-      <c r="G48" s="76"/>
-      <c r="H48" s="76"/>
-      <c r="I48" s="76"/>
-      <c r="J48" s="76"/>
-      <c r="K48" s="76"/>
-      <c r="L48" s="76"/>
-      <c r="M48" s="76"/>
-      <c r="N48" s="76"/>
-      <c r="O48" s="76"/>
-      <c r="P48" s="76"/>
-      <c r="Q48" s="76"/>
+      <c r="A48" s="63"/>
+      <c r="B48" s="63"/>
+      <c r="C48" s="63"/>
+      <c r="D48" s="63"/>
+      <c r="E48" s="63"/>
+      <c r="F48" s="63"/>
+      <c r="G48" s="63"/>
+      <c r="H48" s="63"/>
+      <c r="I48" s="63"/>
+      <c r="J48" s="63"/>
+      <c r="K48" s="63"/>
+      <c r="L48" s="63"/>
+      <c r="M48" s="63"/>
+      <c r="N48" s="63"/>
+      <c r="O48" s="63"/>
+      <c r="P48" s="63"/>
+      <c r="Q48" s="63"/>
     </row>
     <row r="49" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="76"/>
-      <c r="B49" s="76"/>
-      <c r="C49" s="76"/>
-      <c r="D49" s="76"/>
-      <c r="E49" s="76"/>
-      <c r="F49" s="76"/>
-      <c r="G49" s="76"/>
-      <c r="H49" s="76"/>
-      <c r="I49" s="76"/>
-      <c r="J49" s="76"/>
-      <c r="K49" s="76"/>
-      <c r="L49" s="76"/>
-      <c r="M49" s="76"/>
-      <c r="N49" s="76"/>
-      <c r="O49" s="76"/>
-      <c r="P49" s="76"/>
-      <c r="Q49" s="76"/>
+      <c r="A49" s="63"/>
+      <c r="B49" s="63"/>
+      <c r="C49" s="63"/>
+      <c r="D49" s="63"/>
+      <c r="E49" s="63"/>
+      <c r="F49" s="63"/>
+      <c r="G49" s="63"/>
+      <c r="H49" s="63"/>
+      <c r="I49" s="63"/>
+      <c r="J49" s="63"/>
+      <c r="K49" s="63"/>
+      <c r="L49" s="63"/>
+      <c r="M49" s="63"/>
+      <c r="N49" s="63"/>
+      <c r="O49" s="63"/>
+      <c r="P49" s="63"/>
+      <c r="Q49" s="63"/>
     </row>
     <row r="50" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="76"/>
-      <c r="B50" s="76"/>
-      <c r="C50" s="76"/>
-      <c r="D50" s="76"/>
-      <c r="E50" s="76"/>
-      <c r="F50" s="76"/>
-      <c r="G50" s="76"/>
-      <c r="H50" s="76"/>
-      <c r="I50" s="76"/>
-      <c r="J50" s="76"/>
-      <c r="K50" s="76"/>
-      <c r="L50" s="76"/>
-      <c r="M50" s="76"/>
-      <c r="N50" s="76"/>
-      <c r="O50" s="76"/>
-      <c r="P50" s="76"/>
-      <c r="Q50" s="76"/>
+      <c r="A50" s="63"/>
+      <c r="B50" s="63"/>
+      <c r="C50" s="63"/>
+      <c r="D50" s="63"/>
+      <c r="E50" s="63"/>
+      <c r="F50" s="63"/>
+      <c r="G50" s="63"/>
+      <c r="H50" s="63"/>
+      <c r="I50" s="63"/>
+      <c r="J50" s="63"/>
+      <c r="K50" s="63"/>
+      <c r="L50" s="63"/>
+      <c r="M50" s="63"/>
+      <c r="N50" s="63"/>
+      <c r="O50" s="63"/>
+      <c r="P50" s="63"/>
+      <c r="Q50" s="63"/>
     </row>
     <row r="51" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="76"/>
-      <c r="B51" s="76"/>
-      <c r="C51" s="76"/>
-      <c r="D51" s="76"/>
-      <c r="E51" s="76"/>
-      <c r="F51" s="76"/>
-      <c r="G51" s="76"/>
-      <c r="H51" s="76"/>
-      <c r="I51" s="76"/>
-      <c r="J51" s="76"/>
-      <c r="K51" s="76"/>
-      <c r="L51" s="76"/>
-      <c r="M51" s="76"/>
-      <c r="N51" s="76"/>
-      <c r="O51" s="76"/>
-      <c r="P51" s="76"/>
-      <c r="Q51" s="76"/>
+      <c r="A51" s="63"/>
+      <c r="B51" s="63"/>
+      <c r="C51" s="63"/>
+      <c r="D51" s="63"/>
+      <c r="E51" s="63"/>
+      <c r="F51" s="63"/>
+      <c r="G51" s="63"/>
+      <c r="H51" s="63"/>
+      <c r="I51" s="63"/>
+      <c r="J51" s="63"/>
+      <c r="K51" s="63"/>
+      <c r="L51" s="63"/>
+      <c r="M51" s="63"/>
+      <c r="N51" s="63"/>
+      <c r="O51" s="63"/>
+      <c r="P51" s="63"/>
+      <c r="Q51" s="63"/>
     </row>
     <row r="52" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="76"/>
-      <c r="B52" s="76"/>
-      <c r="C52" s="76"/>
-      <c r="D52" s="76"/>
-      <c r="E52" s="76"/>
-      <c r="F52" s="76"/>
-      <c r="G52" s="76"/>
-      <c r="H52" s="76"/>
-      <c r="I52" s="76"/>
-      <c r="J52" s="76"/>
-      <c r="K52" s="76"/>
-      <c r="L52" s="76"/>
-      <c r="M52" s="76"/>
-      <c r="N52" s="76"/>
-      <c r="O52" s="76"/>
-      <c r="P52" s="76"/>
-      <c r="Q52" s="76"/>
+      <c r="A52" s="63"/>
+      <c r="B52" s="63"/>
+      <c r="C52" s="63"/>
+      <c r="D52" s="63"/>
+      <c r="E52" s="63"/>
+      <c r="F52" s="63"/>
+      <c r="G52" s="63"/>
+      <c r="H52" s="63"/>
+      <c r="I52" s="63"/>
+      <c r="J52" s="63"/>
+      <c r="K52" s="63"/>
+      <c r="L52" s="63"/>
+      <c r="M52" s="63"/>
+      <c r="N52" s="63"/>
+      <c r="O52" s="63"/>
+      <c r="P52" s="63"/>
+      <c r="Q52" s="63"/>
     </row>
     <row r="53" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="76"/>
-      <c r="B53" s="76"/>
-      <c r="C53" s="76"/>
-      <c r="D53" s="76"/>
-      <c r="E53" s="76"/>
-      <c r="F53" s="76"/>
-      <c r="G53" s="76"/>
-      <c r="H53" s="76"/>
-      <c r="I53" s="76"/>
-      <c r="J53" s="76"/>
-      <c r="K53" s="76"/>
-      <c r="L53" s="76"/>
-      <c r="M53" s="76"/>
-      <c r="N53" s="76"/>
-      <c r="O53" s="76"/>
-      <c r="P53" s="76"/>
-      <c r="Q53" s="76"/>
+      <c r="A53" s="63"/>
+      <c r="B53" s="63"/>
+      <c r="C53" s="63"/>
+      <c r="D53" s="63"/>
+      <c r="E53" s="63"/>
+      <c r="F53" s="63"/>
+      <c r="G53" s="63"/>
+      <c r="H53" s="63"/>
+      <c r="I53" s="63"/>
+      <c r="J53" s="63"/>
+      <c r="K53" s="63"/>
+      <c r="L53" s="63"/>
+      <c r="M53" s="63"/>
+      <c r="N53" s="63"/>
+      <c r="O53" s="63"/>
+      <c r="P53" s="63"/>
+      <c r="Q53" s="63"/>
     </row>
     <row r="54" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="76"/>
-      <c r="B54" s="76"/>
-      <c r="C54" s="76"/>
-      <c r="D54" s="76"/>
-      <c r="E54" s="76"/>
-      <c r="F54" s="76"/>
-      <c r="G54" s="76"/>
-      <c r="H54" s="76"/>
-      <c r="I54" s="76"/>
-      <c r="J54" s="76"/>
-      <c r="K54" s="76"/>
-      <c r="L54" s="76"/>
-      <c r="M54" s="76"/>
-      <c r="N54" s="76"/>
-      <c r="O54" s="76"/>
-      <c r="P54" s="76"/>
-      <c r="Q54" s="76"/>
+      <c r="A54" s="63"/>
+      <c r="B54" s="63"/>
+      <c r="C54" s="63"/>
+      <c r="D54" s="63"/>
+      <c r="E54" s="63"/>
+      <c r="F54" s="63"/>
+      <c r="G54" s="63"/>
+      <c r="H54" s="63"/>
+      <c r="I54" s="63"/>
+      <c r="J54" s="63"/>
+      <c r="K54" s="63"/>
+      <c r="L54" s="63"/>
+      <c r="M54" s="63"/>
+      <c r="N54" s="63"/>
+      <c r="O54" s="63"/>
+      <c r="P54" s="63"/>
+      <c r="Q54" s="63"/>
     </row>
     <row r="55" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="76"/>
-      <c r="B55" s="76"/>
-      <c r="C55" s="76"/>
-      <c r="D55" s="76"/>
-      <c r="E55" s="76"/>
-      <c r="F55" s="76"/>
-      <c r="G55" s="76"/>
-      <c r="H55" s="76"/>
-      <c r="I55" s="76"/>
-      <c r="J55" s="76"/>
-      <c r="K55" s="76"/>
-      <c r="L55" s="76"/>
-      <c r="M55" s="76"/>
-      <c r="N55" s="76"/>
-      <c r="O55" s="76"/>
-      <c r="P55" s="76"/>
-      <c r="Q55" s="76"/>
+      <c r="A55" s="63"/>
+      <c r="B55" s="63"/>
+      <c r="C55" s="63"/>
+      <c r="D55" s="63"/>
+      <c r="E55" s="63"/>
+      <c r="F55" s="63"/>
+      <c r="G55" s="63"/>
+      <c r="H55" s="63"/>
+      <c r="I55" s="63"/>
+      <c r="J55" s="63"/>
+      <c r="K55" s="63"/>
+      <c r="L55" s="63"/>
+      <c r="M55" s="63"/>
+      <c r="N55" s="63"/>
+      <c r="O55" s="63"/>
+      <c r="P55" s="63"/>
+      <c r="Q55" s="63"/>
     </row>
     <row r="56" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="76"/>
-      <c r="B56" s="76"/>
-      <c r="C56" s="76"/>
-      <c r="D56" s="76"/>
-      <c r="E56" s="76"/>
-      <c r="F56" s="76"/>
-      <c r="G56" s="76"/>
-      <c r="H56" s="76"/>
-      <c r="I56" s="76"/>
-      <c r="J56" s="76"/>
-      <c r="K56" s="76"/>
-      <c r="L56" s="76"/>
-      <c r="M56" s="76"/>
-      <c r="N56" s="76"/>
-      <c r="O56" s="76"/>
-      <c r="P56" s="76"/>
-      <c r="Q56" s="76"/>
+      <c r="A56" s="63"/>
+      <c r="B56" s="63"/>
+      <c r="C56" s="63"/>
+      <c r="D56" s="63"/>
+      <c r="E56" s="63"/>
+      <c r="F56" s="63"/>
+      <c r="G56" s="63"/>
+      <c r="H56" s="63"/>
+      <c r="I56" s="63"/>
+      <c r="J56" s="63"/>
+      <c r="K56" s="63"/>
+      <c r="L56" s="63"/>
+      <c r="M56" s="63"/>
+      <c r="N56" s="63"/>
+      <c r="O56" s="63"/>
+      <c r="P56" s="63"/>
+      <c r="Q56" s="63"/>
     </row>
     <row r="57" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="76"/>
-      <c r="B57" s="76"/>
-      <c r="C57" s="76"/>
-      <c r="D57" s="76"/>
-      <c r="E57" s="76"/>
-      <c r="F57" s="76"/>
-      <c r="G57" s="76"/>
-      <c r="H57" s="76"/>
-      <c r="I57" s="76"/>
-      <c r="J57" s="76"/>
-      <c r="K57" s="76"/>
-      <c r="L57" s="76"/>
-      <c r="M57" s="76"/>
-      <c r="N57" s="76"/>
-      <c r="O57" s="76"/>
-      <c r="P57" s="76"/>
-      <c r="Q57" s="76"/>
+      <c r="A57" s="63"/>
+      <c r="B57" s="63"/>
+      <c r="C57" s="63"/>
+      <c r="D57" s="63"/>
+      <c r="E57" s="63"/>
+      <c r="F57" s="63"/>
+      <c r="G57" s="63"/>
+      <c r="H57" s="63"/>
+      <c r="I57" s="63"/>
+      <c r="J57" s="63"/>
+      <c r="K57" s="63"/>
+      <c r="L57" s="63"/>
+      <c r="M57" s="63"/>
+      <c r="N57" s="63"/>
+      <c r="O57" s="63"/>
+      <c r="P57" s="63"/>
+      <c r="Q57" s="63"/>
     </row>
     <row r="58" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="76"/>
-      <c r="B58" s="76"/>
-      <c r="C58" s="76"/>
-      <c r="D58" s="76"/>
-      <c r="E58" s="76"/>
-      <c r="F58" s="76"/>
-      <c r="G58" s="76"/>
-      <c r="H58" s="76"/>
-      <c r="I58" s="76"/>
-      <c r="J58" s="76"/>
-      <c r="K58" s="76"/>
-      <c r="L58" s="76"/>
-      <c r="M58" s="76"/>
-      <c r="N58" s="76"/>
-      <c r="O58" s="76"/>
-      <c r="P58" s="76"/>
-      <c r="Q58" s="76"/>
+      <c r="A58" s="63"/>
+      <c r="B58" s="63"/>
+      <c r="C58" s="63"/>
+      <c r="D58" s="63"/>
+      <c r="E58" s="63"/>
+      <c r="F58" s="63"/>
+      <c r="G58" s="63"/>
+      <c r="H58" s="63"/>
+      <c r="I58" s="63"/>
+      <c r="J58" s="63"/>
+      <c r="K58" s="63"/>
+      <c r="L58" s="63"/>
+      <c r="M58" s="63"/>
+      <c r="N58" s="63"/>
+      <c r="O58" s="63"/>
+      <c r="P58" s="63"/>
+      <c r="Q58" s="63"/>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A59" s="76"/>
-      <c r="B59" s="76"/>
-      <c r="C59" s="76"/>
-      <c r="D59" s="76"/>
-      <c r="E59" s="76"/>
-      <c r="F59" s="76"/>
-      <c r="G59" s="76"/>
-      <c r="H59" s="76"/>
-      <c r="I59" s="76"/>
-      <c r="J59" s="76"/>
-      <c r="K59" s="76"/>
-      <c r="L59" s="76"/>
-      <c r="M59" s="76"/>
-      <c r="N59" s="76"/>
-      <c r="O59" s="76"/>
-      <c r="P59" s="76"/>
-      <c r="Q59" s="76"/>
+      <c r="A59" s="63"/>
+      <c r="B59" s="63"/>
+      <c r="C59" s="63"/>
+      <c r="D59" s="63"/>
+      <c r="E59" s="63"/>
+      <c r="F59" s="63"/>
+      <c r="G59" s="63"/>
+      <c r="H59" s="63"/>
+      <c r="I59" s="63"/>
+      <c r="J59" s="63"/>
+      <c r="K59" s="63"/>
+      <c r="L59" s="63"/>
+      <c r="M59" s="63"/>
+      <c r="N59" s="63"/>
+      <c r="O59" s="63"/>
+      <c r="P59" s="63"/>
+      <c r="Q59" s="63"/>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A60" s="76"/>
-      <c r="B60" s="76"/>
-      <c r="C60" s="76"/>
-      <c r="D60" s="76"/>
-      <c r="E60" s="76"/>
-      <c r="F60" s="76"/>
-      <c r="G60" s="76"/>
-      <c r="H60" s="76"/>
-      <c r="I60" s="76"/>
-      <c r="J60" s="76"/>
-      <c r="K60" s="76"/>
-      <c r="L60" s="76"/>
-      <c r="M60" s="76"/>
-      <c r="N60" s="76"/>
-      <c r="O60" s="76"/>
-      <c r="P60" s="76"/>
-      <c r="Q60" s="76"/>
+      <c r="A60" s="63"/>
+      <c r="B60" s="63"/>
+      <c r="C60" s="63"/>
+      <c r="D60" s="63"/>
+      <c r="E60" s="63"/>
+      <c r="F60" s="63"/>
+      <c r="G60" s="63"/>
+      <c r="H60" s="63"/>
+      <c r="I60" s="63"/>
+      <c r="J60" s="63"/>
+      <c r="K60" s="63"/>
+      <c r="L60" s="63"/>
+      <c r="M60" s="63"/>
+      <c r="N60" s="63"/>
+      <c r="O60" s="63"/>
+      <c r="P60" s="63"/>
+      <c r="Q60" s="63"/>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A61" s="76"/>
-      <c r="B61" s="76"/>
-      <c r="C61" s="76"/>
-      <c r="D61" s="76"/>
-      <c r="E61" s="76"/>
-      <c r="F61" s="76"/>
-      <c r="G61" s="76"/>
-      <c r="H61" s="76"/>
-      <c r="I61" s="76"/>
-      <c r="J61" s="76"/>
-      <c r="K61" s="76"/>
-      <c r="L61" s="76"/>
-      <c r="M61" s="76"/>
-      <c r="N61" s="76"/>
-      <c r="O61" s="76"/>
-      <c r="P61" s="76"/>
-      <c r="Q61" s="76"/>
+      <c r="A61" s="63"/>
+      <c r="B61" s="63"/>
+      <c r="C61" s="63"/>
+      <c r="D61" s="63"/>
+      <c r="E61" s="63"/>
+      <c r="F61" s="63"/>
+      <c r="G61" s="63"/>
+      <c r="H61" s="63"/>
+      <c r="I61" s="63"/>
+      <c r="J61" s="63"/>
+      <c r="K61" s="63"/>
+      <c r="L61" s="63"/>
+      <c r="M61" s="63"/>
+      <c r="N61" s="63"/>
+      <c r="O61" s="63"/>
+      <c r="P61" s="63"/>
+      <c r="Q61" s="63"/>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A62" s="76"/>
-      <c r="B62" s="76"/>
-      <c r="C62" s="76"/>
-      <c r="D62" s="76"/>
-      <c r="E62" s="76"/>
-      <c r="F62" s="76"/>
-      <c r="G62" s="76"/>
-      <c r="H62" s="76"/>
-      <c r="I62" s="76"/>
-      <c r="J62" s="76"/>
-      <c r="K62" s="76"/>
-      <c r="L62" s="76"/>
-      <c r="M62" s="76"/>
-      <c r="N62" s="76"/>
-      <c r="O62" s="76"/>
-      <c r="P62" s="76"/>
-      <c r="Q62" s="76"/>
+      <c r="A62" s="63"/>
+      <c r="B62" s="63"/>
+      <c r="C62" s="63"/>
+      <c r="D62" s="63"/>
+      <c r="E62" s="63"/>
+      <c r="F62" s="63"/>
+      <c r="G62" s="63"/>
+      <c r="H62" s="63"/>
+      <c r="I62" s="63"/>
+      <c r="J62" s="63"/>
+      <c r="K62" s="63"/>
+      <c r="L62" s="63"/>
+      <c r="M62" s="63"/>
+      <c r="N62" s="63"/>
+      <c r="O62" s="63"/>
+      <c r="P62" s="63"/>
+      <c r="Q62" s="63"/>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A63" s="76"/>
-      <c r="B63" s="76"/>
-      <c r="C63" s="76"/>
-      <c r="D63" s="76"/>
-      <c r="E63" s="76"/>
-      <c r="F63" s="76"/>
-      <c r="G63" s="76"/>
-      <c r="H63" s="76"/>
-      <c r="I63" s="76"/>
-      <c r="J63" s="76"/>
-      <c r="K63" s="76"/>
-      <c r="L63" s="76"/>
-      <c r="M63" s="76"/>
-      <c r="N63" s="76"/>
-      <c r="O63" s="76"/>
-      <c r="P63" s="76"/>
-      <c r="Q63" s="76"/>
+      <c r="A63" s="63"/>
+      <c r="B63" s="63"/>
+      <c r="C63" s="63"/>
+      <c r="D63" s="63"/>
+      <c r="E63" s="63"/>
+      <c r="F63" s="63"/>
+      <c r="G63" s="63"/>
+      <c r="H63" s="63"/>
+      <c r="I63" s="63"/>
+      <c r="J63" s="63"/>
+      <c r="K63" s="63"/>
+      <c r="L63" s="63"/>
+      <c r="M63" s="63"/>
+      <c r="N63" s="63"/>
+      <c r="O63" s="63"/>
+      <c r="P63" s="63"/>
+      <c r="Q63" s="63"/>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A64" s="76"/>
-      <c r="B64" s="76"/>
-      <c r="C64" s="76"/>
-      <c r="D64" s="76"/>
-      <c r="E64" s="76"/>
-      <c r="F64" s="76"/>
-      <c r="G64" s="76"/>
-      <c r="H64" s="76"/>
-      <c r="I64" s="76"/>
-      <c r="J64" s="76"/>
-      <c r="K64" s="76"/>
-      <c r="L64" s="76"/>
-      <c r="M64" s="76"/>
-      <c r="N64" s="76"/>
-      <c r="O64" s="76"/>
-      <c r="P64" s="76"/>
-      <c r="Q64" s="76"/>
+      <c r="A64" s="63"/>
+      <c r="B64" s="63"/>
+      <c r="C64" s="63"/>
+      <c r="D64" s="63"/>
+      <c r="E64" s="63"/>
+      <c r="F64" s="63"/>
+      <c r="G64" s="63"/>
+      <c r="H64" s="63"/>
+      <c r="I64" s="63"/>
+      <c r="J64" s="63"/>
+      <c r="K64" s="63"/>
+      <c r="L64" s="63"/>
+      <c r="M64" s="63"/>
+      <c r="N64" s="63"/>
+      <c r="O64" s="63"/>
+      <c r="P64" s="63"/>
+      <c r="Q64" s="63"/>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A65" s="76"/>
-      <c r="B65" s="76"/>
-      <c r="C65" s="76"/>
-      <c r="D65" s="76"/>
-      <c r="E65" s="76"/>
-      <c r="F65" s="76"/>
-      <c r="G65" s="76"/>
-      <c r="H65" s="76"/>
-      <c r="I65" s="76"/>
-      <c r="J65" s="76"/>
-      <c r="K65" s="76"/>
-      <c r="L65" s="76"/>
-      <c r="M65" s="76"/>
-      <c r="N65" s="76"/>
-      <c r="O65" s="76"/>
-      <c r="P65" s="76"/>
-      <c r="Q65" s="76"/>
+      <c r="A65" s="63"/>
+      <c r="B65" s="63"/>
+      <c r="C65" s="63"/>
+      <c r="D65" s="63"/>
+      <c r="E65" s="63"/>
+      <c r="F65" s="63"/>
+      <c r="G65" s="63"/>
+      <c r="H65" s="63"/>
+      <c r="I65" s="63"/>
+      <c r="J65" s="63"/>
+      <c r="K65" s="63"/>
+      <c r="L65" s="63"/>
+      <c r="M65" s="63"/>
+      <c r="N65" s="63"/>
+      <c r="O65" s="63"/>
+      <c r="P65" s="63"/>
+      <c r="Q65" s="63"/>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A66" s="76"/>
-      <c r="B66" s="76"/>
-      <c r="C66" s="76"/>
-      <c r="D66" s="76"/>
-      <c r="E66" s="76"/>
-      <c r="F66" s="76"/>
-      <c r="G66" s="76"/>
-      <c r="H66" s="76"/>
-      <c r="I66" s="76"/>
-      <c r="J66" s="76"/>
-      <c r="K66" s="76"/>
-      <c r="L66" s="76"/>
-      <c r="M66" s="76"/>
-      <c r="N66" s="76"/>
-      <c r="O66" s="76"/>
-      <c r="P66" s="76"/>
-      <c r="Q66" s="76"/>
+      <c r="A66" s="63"/>
+      <c r="B66" s="63"/>
+      <c r="C66" s="63"/>
+      <c r="D66" s="63"/>
+      <c r="E66" s="63"/>
+      <c r="F66" s="63"/>
+      <c r="G66" s="63"/>
+      <c r="H66" s="63"/>
+      <c r="I66" s="63"/>
+      <c r="J66" s="63"/>
+      <c r="K66" s="63"/>
+      <c r="L66" s="63"/>
+      <c r="M66" s="63"/>
+      <c r="N66" s="63"/>
+      <c r="O66" s="63"/>
+      <c r="P66" s="63"/>
+      <c r="Q66" s="63"/>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A67" s="76"/>
-      <c r="B67" s="76"/>
-      <c r="C67" s="76"/>
-      <c r="D67" s="76"/>
-      <c r="E67" s="76"/>
-      <c r="F67" s="76"/>
-      <c r="G67" s="76"/>
-      <c r="H67" s="76"/>
-      <c r="I67" s="76"/>
-      <c r="J67" s="76"/>
-      <c r="K67" s="76"/>
-      <c r="L67" s="76"/>
-      <c r="M67" s="76"/>
-      <c r="N67" s="76"/>
-      <c r="O67" s="76"/>
-      <c r="P67" s="76"/>
-      <c r="Q67" s="76"/>
+      <c r="A67" s="63"/>
+      <c r="B67" s="63"/>
+      <c r="C67" s="63"/>
+      <c r="D67" s="63"/>
+      <c r="E67" s="63"/>
+      <c r="F67" s="63"/>
+      <c r="G67" s="63"/>
+      <c r="H67" s="63"/>
+      <c r="I67" s="63"/>
+      <c r="J67" s="63"/>
+      <c r="K67" s="63"/>
+      <c r="L67" s="63"/>
+      <c r="M67" s="63"/>
+      <c r="N67" s="63"/>
+      <c r="O67" s="63"/>
+      <c r="P67" s="63"/>
+      <c r="Q67" s="63"/>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A68" s="76"/>
-      <c r="B68" s="76"/>
-      <c r="C68" s="76"/>
-      <c r="D68" s="76"/>
-      <c r="E68" s="76"/>
-      <c r="F68" s="76"/>
-      <c r="G68" s="76"/>
-      <c r="H68" s="76"/>
-      <c r="I68" s="76"/>
-      <c r="J68" s="76"/>
-      <c r="K68" s="76"/>
-      <c r="L68" s="76"/>
-      <c r="M68" s="76"/>
-      <c r="N68" s="76"/>
-      <c r="O68" s="76"/>
-      <c r="P68" s="76"/>
-      <c r="Q68" s="76"/>
+      <c r="A68" s="63"/>
+      <c r="B68" s="63"/>
+      <c r="C68" s="63"/>
+      <c r="D68" s="63"/>
+      <c r="E68" s="63"/>
+      <c r="F68" s="63"/>
+      <c r="G68" s="63"/>
+      <c r="H68" s="63"/>
+      <c r="I68" s="63"/>
+      <c r="J68" s="63"/>
+      <c r="K68" s="63"/>
+      <c r="L68" s="63"/>
+      <c r="M68" s="63"/>
+      <c r="N68" s="63"/>
+      <c r="O68" s="63"/>
+      <c r="P68" s="63"/>
+      <c r="Q68" s="63"/>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A69" s="76"/>
-      <c r="B69" s="76"/>
-      <c r="C69" s="76"/>
-      <c r="D69" s="76"/>
-      <c r="E69" s="76"/>
-      <c r="F69" s="76"/>
-      <c r="G69" s="76"/>
-      <c r="H69" s="76"/>
-      <c r="I69" s="76"/>
-      <c r="J69" s="76"/>
-      <c r="K69" s="76"/>
-      <c r="L69" s="76"/>
-      <c r="M69" s="76"/>
-      <c r="N69" s="76"/>
-      <c r="O69" s="76"/>
-      <c r="P69" s="76"/>
-      <c r="Q69" s="76"/>
+      <c r="A69" s="63"/>
+      <c r="B69" s="63"/>
+      <c r="C69" s="63"/>
+      <c r="D69" s="63"/>
+      <c r="E69" s="63"/>
+      <c r="F69" s="63"/>
+      <c r="G69" s="63"/>
+      <c r="H69" s="63"/>
+      <c r="I69" s="63"/>
+      <c r="J69" s="63"/>
+      <c r="K69" s="63"/>
+      <c r="L69" s="63"/>
+      <c r="M69" s="63"/>
+      <c r="N69" s="63"/>
+      <c r="O69" s="63"/>
+      <c r="P69" s="63"/>
+      <c r="Q69" s="63"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A70" s="76"/>
-      <c r="B70" s="76"/>
-      <c r="C70" s="76"/>
-      <c r="D70" s="76"/>
-      <c r="E70" s="76"/>
-      <c r="F70" s="76"/>
-      <c r="G70" s="76"/>
-      <c r="H70" s="76"/>
-      <c r="I70" s="76"/>
-      <c r="J70" s="76"/>
-      <c r="K70" s="76"/>
-      <c r="L70" s="76"/>
-      <c r="M70" s="76"/>
-      <c r="N70" s="76"/>
-      <c r="O70" s="76"/>
-      <c r="P70" s="76"/>
-      <c r="Q70" s="76"/>
+      <c r="A70" s="63"/>
+      <c r="B70" s="63"/>
+      <c r="C70" s="63"/>
+      <c r="D70" s="63"/>
+      <c r="E70" s="63"/>
+      <c r="F70" s="63"/>
+      <c r="G70" s="63"/>
+      <c r="H70" s="63"/>
+      <c r="I70" s="63"/>
+      <c r="J70" s="63"/>
+      <c r="K70" s="63"/>
+      <c r="L70" s="63"/>
+      <c r="M70" s="63"/>
+      <c r="N70" s="63"/>
+      <c r="O70" s="63"/>
+      <c r="P70" s="63"/>
+      <c r="Q70" s="63"/>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A71" s="76"/>
-      <c r="B71" s="76"/>
-      <c r="C71" s="76"/>
-      <c r="D71" s="76"/>
-      <c r="E71" s="76"/>
-      <c r="F71" s="76"/>
-      <c r="G71" s="76"/>
-      <c r="H71" s="76"/>
-      <c r="I71" s="76"/>
-      <c r="J71" s="76"/>
-      <c r="K71" s="76"/>
-      <c r="L71" s="76"/>
-      <c r="M71" s="76"/>
-      <c r="N71" s="76"/>
-      <c r="O71" s="76"/>
-      <c r="P71" s="76"/>
-      <c r="Q71" s="76"/>
+      <c r="A71" s="63"/>
+      <c r="B71" s="63"/>
+      <c r="C71" s="63"/>
+      <c r="D71" s="63"/>
+      <c r="E71" s="63"/>
+      <c r="F71" s="63"/>
+      <c r="G71" s="63"/>
+      <c r="H71" s="63"/>
+      <c r="I71" s="63"/>
+      <c r="J71" s="63"/>
+      <c r="K71" s="63"/>
+      <c r="L71" s="63"/>
+      <c r="M71" s="63"/>
+      <c r="N71" s="63"/>
+      <c r="O71" s="63"/>
+      <c r="P71" s="63"/>
+      <c r="Q71" s="63"/>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A72" s="76"/>
-      <c r="B72" s="76"/>
-      <c r="C72" s="76"/>
-      <c r="D72" s="76"/>
-      <c r="E72" s="76"/>
-      <c r="F72" s="76"/>
-      <c r="G72" s="76"/>
-      <c r="H72" s="76"/>
-      <c r="I72" s="76"/>
-      <c r="J72" s="76"/>
-      <c r="K72" s="76"/>
-      <c r="L72" s="76"/>
-      <c r="M72" s="76"/>
-      <c r="N72" s="76"/>
-      <c r="O72" s="76"/>
-      <c r="P72" s="76"/>
-      <c r="Q72" s="76"/>
+      <c r="A72" s="63"/>
+      <c r="B72" s="63"/>
+      <c r="C72" s="63"/>
+      <c r="D72" s="63"/>
+      <c r="E72" s="63"/>
+      <c r="F72" s="63"/>
+      <c r="G72" s="63"/>
+      <c r="H72" s="63"/>
+      <c r="I72" s="63"/>
+      <c r="J72" s="63"/>
+      <c r="K72" s="63"/>
+      <c r="L72" s="63"/>
+      <c r="M72" s="63"/>
+      <c r="N72" s="63"/>
+      <c r="O72" s="63"/>
+      <c r="P72" s="63"/>
+      <c r="Q72" s="63"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="TvzJA4dj5gAiAqMN3NmS+yF72Cf9cZxll9cugNRhLgW/PtoxYzSvLU7DNKYpAAZE3kgpn9982NVwAUY7NHCuIg==" saltValue="fwhso3I15m4r0J9MlePHUg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="xRuQTCt2Mfn3PZYGHNZedrp6E1Fua6jF+pb/3RGPl6cSldacVBNRr+D27sPG9cbi9TnOrk3M6cSHaSLlGCqOaA==" saltValue="s+XQoa420GaEnFPERKc1qg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="B1 D1" name="Range1_28"/>
     <protectedRange sqref="F10:G13 I10:J13 L10:M13 C10:D13 C14:Q14 O10:P13 C15:D16 F15:G16 I15:J16 L15:M16 O15:P16 C6:D8 F6:G8 I6:J8 L6:M8 O6:P8" name="Range1_28_1"/>
   </protectedRanges>
   <mergeCells count="22">
+    <mergeCell ref="C3:E4"/>
+    <mergeCell ref="F3:H4"/>
+    <mergeCell ref="I3:K4"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
     <mergeCell ref="O2:Q2"/>
     <mergeCell ref="O3:Q4"/>
     <mergeCell ref="A28:Q72"/>
@@ -4646,29 +4664,23 @@
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="C2:K2"/>
     <mergeCell ref="L2:N2"/>
-    <mergeCell ref="C3:E4"/>
-    <mergeCell ref="F3:H4"/>
-    <mergeCell ref="I3:K4"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
   </mergeCells>
-  <conditionalFormatting sqref="E6:E8 E10:E16">
+  <conditionalFormatting sqref="E10:E16 E6:E8">
     <cfRule type="cellIs" dxfId="96" priority="66" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H6:H8 H10:H16">
+  <conditionalFormatting sqref="H10:H16 H6:H8">
     <cfRule type="cellIs" dxfId="95" priority="65" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6:K8 K10:K16">
+  <conditionalFormatting sqref="K10:K16 K6:K8">
     <cfRule type="cellIs" dxfId="94" priority="64" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N7:N8 N10:N16">
+  <conditionalFormatting sqref="N10:N16 N6:N8">
     <cfRule type="cellIs" dxfId="93" priority="63" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -4929,7 +4941,7 @@
       <selection activeCell="F2" sqref="F2:H2"/>
       <selection pane="topRight" activeCell="F2" sqref="F2:H2"/>
       <selection pane="bottomLeft" activeCell="F2" sqref="F2:H2"/>
-      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4951,109 +4963,109 @@
       <c r="A1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="47"/>
+      <c r="B1" s="46"/>
       <c r="C1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="53"/>
+      <c r="D1" s="52"/>
       <c r="E1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="53">
+      <c r="F1" s="52">
         <v>10</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="82">
+      <c r="H1" s="70">
         <v>2019</v>
       </c>
-      <c r="I1" s="83"/>
-      <c r="J1" s="100" t="s">
+      <c r="I1" s="71"/>
+      <c r="J1" s="92" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="101"/>
-      <c r="L1" s="101"/>
-      <c r="M1" s="102" t="str">
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="94" t="str">
         <f>IF(COUNTIF(O20:O25,"&lt;&gt;0"),"Report has Errors","Report is Correct")</f>
         <v>Report is Correct</v>
       </c>
-      <c r="N1" s="103"/>
+      <c r="N1" s="95"/>
     </row>
     <row r="2" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="104" t="s">
+      <c r="A2" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="89" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="92" t="s">
+      <c r="B2" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="67" t="s">
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="68"/>
-      <c r="N2" s="69"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="56"/>
     </row>
     <row r="3" spans="1:17" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="92"/>
-      <c r="B3" s="90"/>
-      <c r="C3" s="55" t="s">
+      <c r="A3" s="80"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="55" t="s">
+      <c r="D3" s="82"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="56"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="55" t="s">
+      <c r="G3" s="82"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="56"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="70" t="s">
+      <c r="J3" s="82"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="M3" s="71"/>
-      <c r="N3" s="72"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="59"/>
     </row>
     <row r="4" spans="1:17" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="92"/>
-      <c r="B4" s="90"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="63"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="74"/>
-      <c r="N4" s="75"/>
+      <c r="A4" s="80"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="62"/>
     </row>
     <row r="5" spans="1:17" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="92"/>
-      <c r="B5" s="91"/>
-      <c r="C5" s="23" t="s">
+      <c r="A5" s="80"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="24" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="19" t="s">
@@ -5083,14 +5095,14 @@
       <c r="N5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="O5" s="33"/>
-      <c r="Q5" s="33"/>
+      <c r="O5" s="32"/>
+      <c r="Q5" s="32"/>
     </row>
     <row r="6" spans="1:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="14"/>
@@ -5119,10 +5131,10 @@
       </c>
     </row>
     <row r="7" spans="1:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="34" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="14"/>
@@ -5165,10 +5177,10 @@
       </c>
     </row>
     <row r="8" spans="1:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="34" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="14"/>
@@ -5211,10 +5223,10 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="34" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="4">
@@ -5267,10 +5279,10 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="14"/>
@@ -5313,10 +5325,10 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="34" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="14">
@@ -5361,10 +5373,10 @@
       </c>
     </row>
     <row r="12" spans="1:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="34" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="14">
@@ -5409,10 +5421,10 @@
       </c>
     </row>
     <row r="13" spans="1:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="34" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="14"/>
@@ -5451,17 +5463,17 @@
       </c>
     </row>
     <row r="14" spans="1:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="34" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="4">
         <f>C9-SUM(C10:C13)</f>
         <v>0</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="25">
         <f>D9-SUM(D10:D13)</f>
         <v>0</v>
       </c>
@@ -5469,11 +5481,11 @@
         <f t="shared" ref="E14:N14" si="5">E9-SUM(E10:E13)</f>
         <v>0</v>
       </c>
-      <c r="F14" s="26">
+      <c r="F14" s="25">
         <f>F9-SUM(F10:F13)</f>
         <v>0</v>
       </c>
-      <c r="G14" s="26">
+      <c r="G14" s="25">
         <f>G9-SUM(G10:G13)</f>
         <v>0</v>
       </c>
@@ -5481,11 +5493,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I14" s="26">
+      <c r="I14" s="25">
         <f>I9-SUM(I10:I13)</f>
         <v>0</v>
       </c>
-      <c r="J14" s="26">
+      <c r="J14" s="25">
         <f>J9-SUM(J10:J13)</f>
         <v>0</v>
       </c>
@@ -5493,11 +5505,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="L14" s="26">
+      <c r="L14" s="25">
         <f>L9-SUM(L10:L13)</f>
         <v>0</v>
       </c>
-      <c r="M14" s="26">
+      <c r="M14" s="25">
         <f>M9-SUM(M10:M13)</f>
         <v>0</v>
       </c>
@@ -5507,10 +5519,10 @@
       </c>
     </row>
     <row r="15" spans="1:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="34" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="14"/>
@@ -5539,98 +5551,98 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="41">
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="41">
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="41">
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L16" s="40"/>
-      <c r="M16" s="40"/>
-      <c r="N16" s="41">
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="40">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="43" t="str">
+      <c r="C17" s="42" t="str">
         <f>IFERROR(C14/C9,"")</f>
         <v/>
       </c>
-      <c r="D17" s="44" t="str">
+      <c r="D17" s="43" t="str">
         <f t="shared" ref="D17:N17" si="6">IFERROR(D14/D9,"")</f>
         <v/>
       </c>
-      <c r="E17" s="45" t="str">
+      <c r="E17" s="44" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F17" s="43" t="str">
+      <c r="F17" s="42" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="G17" s="44" t="str">
+      <c r="G17" s="43" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="H17" s="45" t="str">
+      <c r="H17" s="44" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I17" s="43" t="str">
+      <c r="I17" s="42" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="J17" s="44" t="str">
+      <c r="J17" s="43" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="K17" s="45" t="str">
+      <c r="K17" s="44" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="L17" s="43" t="str">
+      <c r="L17" s="42" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="M17" s="44" t="str">
+      <c r="M17" s="43" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="N17" s="45" t="str">
+      <c r="N17" s="44" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:15" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="45" t="s">
         <v>31</v>
       </c>
       <c r="C18" s="6" t="str">
@@ -5683,705 +5695,705 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="20.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="95" t="s">
+      <c r="A19" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="96"/>
-      <c r="C19" s="96"/>
-      <c r="D19" s="96"/>
-      <c r="E19" s="96"/>
-      <c r="F19" s="96"/>
-      <c r="G19" s="96"/>
-      <c r="H19" s="96"/>
-      <c r="I19" s="96"/>
-      <c r="J19" s="96"/>
-      <c r="K19" s="96"/>
-      <c r="L19" s="96"/>
-      <c r="M19" s="96"/>
-      <c r="N19" s="97"/>
+      <c r="B19" s="100"/>
+      <c r="C19" s="100"/>
+      <c r="D19" s="100"/>
+      <c r="E19" s="100"/>
+      <c r="F19" s="100"/>
+      <c r="G19" s="100"/>
+      <c r="H19" s="100"/>
+      <c r="I19" s="100"/>
+      <c r="J19" s="100"/>
+      <c r="K19" s="100"/>
+      <c r="L19" s="100"/>
+      <c r="M19" s="100"/>
+      <c r="N19" s="101"/>
     </row>
     <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="93" t="s">
+      <c r="A20" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="93"/>
-      <c r="C20" s="27">
+      <c r="B20" s="97"/>
+      <c r="C20" s="26">
         <f>C14</f>
         <v>0</v>
       </c>
-      <c r="D20" s="27">
+      <c r="D20" s="26">
         <f>D14</f>
         <v>0</v>
       </c>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27">
+      <c r="E20" s="26"/>
+      <c r="F20" s="26">
         <f>F14</f>
         <v>0</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G20" s="26">
         <f>G14</f>
         <v>0</v>
       </c>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27">
+      <c r="H20" s="26"/>
+      <c r="I20" s="26">
         <f>I14</f>
         <v>0</v>
       </c>
-      <c r="J20" s="27">
+      <c r="J20" s="26">
         <f>J14</f>
         <v>0</v>
       </c>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27">
+      <c r="K20" s="26"/>
+      <c r="L20" s="26">
         <f>L14</f>
         <v>0</v>
       </c>
-      <c r="M20" s="27">
+      <c r="M20" s="26">
         <f>M14</f>
         <v>0</v>
       </c>
-      <c r="N20" s="27"/>
-      <c r="O20" s="27">
+      <c r="N20" s="26"/>
+      <c r="O20" s="26">
         <f>COUNTIF(C20:N20,"&lt;0")</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="93" t="s">
+      <c r="A21" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="93"/>
-      <c r="C21" s="27">
+      <c r="B21" s="97"/>
+      <c r="C21" s="26">
         <f>C15-C16</f>
         <v>0</v>
       </c>
-      <c r="D21" s="27">
+      <c r="D21" s="26">
         <f>D15-D16</f>
         <v>0</v>
       </c>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27">
+      <c r="E21" s="26"/>
+      <c r="F21" s="26">
         <f>F15-F16</f>
         <v>0</v>
       </c>
-      <c r="G21" s="27">
+      <c r="G21" s="26">
         <f>G15-G16</f>
         <v>0</v>
       </c>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27">
+      <c r="H21" s="26"/>
+      <c r="I21" s="26">
         <f>I15-I16</f>
         <v>0</v>
       </c>
-      <c r="J21" s="27">
+      <c r="J21" s="26">
         <f>J15-J16</f>
         <v>0</v>
       </c>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27">
+      <c r="K21" s="26"/>
+      <c r="L21" s="26">
         <f>L15-L16</f>
         <v>0</v>
       </c>
-      <c r="M21" s="27">
+      <c r="M21" s="26">
         <f>M15-M16</f>
         <v>0</v>
       </c>
-      <c r="N21" s="27"/>
-      <c r="O21" s="27">
+      <c r="N21" s="26"/>
+      <c r="O21" s="26">
         <f t="shared" ref="O21:O25" si="8">COUNTIF(C21:N21,"&lt;0")</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="93" t="s">
+      <c r="A22" s="97" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="93"/>
-      <c r="C22" s="32" t="str">
+      <c r="B22" s="97"/>
+      <c r="C22" s="31" t="str">
         <f>IF(C20&lt;0,C$26&amp;"  Has "&amp;$A22,"")</f>
         <v/>
       </c>
-      <c r="D22" s="32" t="str">
+      <c r="D22" s="31" t="str">
         <f t="shared" ref="D22:N23" si="9">IF(D20&lt;0,D$26&amp;"  Has "&amp;$A22,"")</f>
         <v/>
       </c>
-      <c r="E22" s="32" t="str">
+      <c r="E22" s="31" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="F22" s="32" t="str">
+      <c r="F22" s="31" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G22" s="32" t="str">
+      <c r="G22" s="31" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="H22" s="32" t="str">
+      <c r="H22" s="31" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="I22" s="32" t="str">
+      <c r="I22" s="31" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="J22" s="32" t="str">
+      <c r="J22" s="31" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="K22" s="32" t="str">
+      <c r="K22" s="31" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="L22" s="32" t="str">
+      <c r="L22" s="31" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="M22" s="32" t="str">
+      <c r="M22" s="31" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="N22" s="32" t="str">
+      <c r="N22" s="31" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="O22" s="50">
+      <c r="O22" s="49">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="93" t="s">
+      <c r="A23" s="97" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="93"/>
-      <c r="C23" s="32" t="str">
+      <c r="B23" s="97"/>
+      <c r="C23" s="31" t="str">
         <f>IF(C21&lt;0,C$26&amp;"  Has "&amp;$A23,"")</f>
         <v/>
       </c>
-      <c r="D23" s="32" t="str">
+      <c r="D23" s="31" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="E23" s="32" t="str">
+      <c r="E23" s="31" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="F23" s="32" t="str">
+      <c r="F23" s="31" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="G23" s="32" t="str">
+      <c r="G23" s="31" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="H23" s="32" t="str">
+      <c r="H23" s="31" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="I23" s="32" t="str">
+      <c r="I23" s="31" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="J23" s="32" t="str">
+      <c r="J23" s="31" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="K23" s="32" t="str">
+      <c r="K23" s="31" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="L23" s="32" t="str">
+      <c r="L23" s="31" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="M23" s="32" t="str">
+      <c r="M23" s="31" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="N23" s="32" t="str">
+      <c r="N23" s="31" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="O23" s="50">
+      <c r="O23" s="49">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="98" t="s">
+      <c r="A24" s="102" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="98"/>
-      <c r="C24" s="52">
-        <f>C6-F6-I6</f>
-        <v>0</v>
-      </c>
-      <c r="D24" s="52">
-        <f>D6-G6-J6</f>
-        <v>0</v>
-      </c>
-      <c r="E24" s="52">
+      <c r="B24" s="102"/>
+      <c r="C24" s="104">
+        <f>(C6-F6)-(F6-I6)</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="104">
+        <f>(D6-G6)-(G6-J6)</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="51">
         <f>IF(C24&lt;&gt;0,-1,IF(D24&lt;&gt;0,-1,0))</f>
         <v>0</v>
       </c>
-      <c r="F24" s="52"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="52"/>
-      <c r="L24" s="52"/>
-      <c r="M24" s="52"/>
-      <c r="N24" s="52"/>
-      <c r="O24" s="50">
+      <c r="F24" s="51"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="51"/>
+      <c r="L24" s="51"/>
+      <c r="M24" s="51"/>
+      <c r="N24" s="51"/>
+      <c r="O24" s="49">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="99" t="s">
+      <c r="A25" s="103" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="99"/>
-      <c r="C25" s="52">
+      <c r="B25" s="103"/>
+      <c r="C25" s="51">
         <f>C14-C15</f>
         <v>0</v>
       </c>
-      <c r="D25" s="52">
+      <c r="D25" s="51">
         <f t="shared" ref="D25:M25" si="10">D14-D15</f>
         <v>0</v>
       </c>
-      <c r="E25" s="52"/>
-      <c r="F25" s="52">
+      <c r="E25" s="51"/>
+      <c r="F25" s="51">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="G25" s="52">
+      <c r="G25" s="51">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="H25" s="52"/>
-      <c r="I25" s="52">
+      <c r="H25" s="51"/>
+      <c r="I25" s="51">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="J25" s="52">
+      <c r="J25" s="51">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="K25" s="52"/>
-      <c r="L25" s="52">
+      <c r="K25" s="51"/>
+      <c r="L25" s="51">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M25" s="52">
+      <c r="M25" s="51">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="N25" s="52"/>
-      <c r="O25" s="50">
+      <c r="N25" s="51"/>
+      <c r="O25" s="49">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="64" t="s">
+    <row r="26" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="90" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="64"/>
-      <c r="C26" s="32" t="str">
+      <c r="B26" s="90"/>
+      <c r="C26" s="31" t="str">
         <f>$C3&amp;" "&amp;C5</f>
         <v>3 months cohort Known Positive</v>
       </c>
-      <c r="D26" s="32" t="str">
+      <c r="D26" s="31" t="str">
         <f>$C3&amp;" "&amp;D5</f>
         <v>3 months cohort New Positive</v>
       </c>
-      <c r="E26" s="32" t="str">
+      <c r="E26" s="31" t="str">
         <f>$C3&amp;" "&amp;E5</f>
         <v>3 months cohort Total</v>
       </c>
-      <c r="F26" s="32" t="str">
+      <c r="F26" s="31" t="str">
         <f>$F3&amp;" "&amp;F5</f>
         <v>6 months cohort Known Positive</v>
       </c>
-      <c r="G26" s="32" t="str">
+      <c r="G26" s="31" t="str">
         <f>$F3&amp;" "&amp;G5</f>
         <v>6 months cohort New Positive</v>
       </c>
-      <c r="H26" s="32" t="str">
+      <c r="H26" s="31" t="str">
         <f>$F3&amp;" "&amp;H5</f>
         <v>6 months cohort Total</v>
       </c>
-      <c r="I26" s="32" t="str">
+      <c r="I26" s="31" t="str">
         <f>$I3&amp;" "&amp;I5</f>
         <v>12 months cohort Known Positive</v>
       </c>
-      <c r="J26" s="32" t="str">
+      <c r="J26" s="31" t="str">
         <f t="shared" ref="J26:K26" si="11">$I3&amp;" "&amp;J5</f>
         <v>12 months cohort New Positive</v>
       </c>
-      <c r="K26" s="32" t="str">
+      <c r="K26" s="31" t="str">
         <f t="shared" si="11"/>
         <v>12 months cohort Total</v>
       </c>
-      <c r="L26" s="32" t="str">
+      <c r="L26" s="31" t="str">
         <f>$L3&amp;" "&amp;L5</f>
         <v>24 months cohort Known Positive</v>
       </c>
-      <c r="M26" s="32" t="str">
+      <c r="M26" s="31" t="str">
         <f>$L3&amp;" "&amp;M5</f>
         <v>24 months cohort New Positive</v>
       </c>
-      <c r="N26" s="32" t="str">
+      <c r="N26" s="31" t="str">
         <f>$L3&amp;" "&amp;N5</f>
         <v>24 months cohort Total</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="94" t="str">
+      <c r="A28" s="98" t="str">
         <f>C22&amp;CHAR(10) &amp;D22 &amp;CHAR(10) &amp;E22 &amp;CHAR(10) &amp;F22 &amp; CHAR( 10 ) &amp;G22 &amp; CHAR( 10 ) &amp;H22 &amp; CHAR( 10 ) &amp;I22 &amp; CHAR( 10 ) &amp;J22 &amp; CHAR( 10 ) &amp;K22 &amp; CHAR( 10 ) &amp;L22 &amp; CHAR( 10 ) &amp;M22 &amp; CHAR( 10 ) &amp;N22 &amp; CHAR( 10 ) &amp;C23 &amp; CHAR( 10 ) &amp;D23 &amp; CHAR( 10 ) &amp;E23 &amp; CHAR( 10 ) &amp;F23 &amp; CHAR( 10 ) &amp;G23 &amp; CHAR( 10 ) &amp;H23 &amp; CHAR( 10 ) &amp;I23 &amp; CHAR( 10 ) &amp;J23 &amp; CHAR( 10 ) &amp;K23 &amp; CHAR( 10 ) &amp;L23 &amp; CHAR( 10 ) &amp;M23 &amp; CHAR( 10 ) &amp;N23</f>
         <v xml:space="preserve">
 </v>
       </c>
-      <c r="B28" s="94"/>
-      <c r="C28" s="94"/>
-      <c r="D28" s="94"/>
-      <c r="E28" s="94"/>
-      <c r="F28" s="94"/>
-      <c r="G28" s="94"/>
-      <c r="H28" s="94"/>
-      <c r="I28" s="94"/>
-      <c r="J28" s="94"/>
-      <c r="K28" s="94"/>
-      <c r="L28" s="94"/>
-      <c r="M28" s="94"/>
-      <c r="N28" s="94"/>
+      <c r="B28" s="98"/>
+      <c r="C28" s="98"/>
+      <c r="D28" s="98"/>
+      <c r="E28" s="98"/>
+      <c r="F28" s="98"/>
+      <c r="G28" s="98"/>
+      <c r="H28" s="98"/>
+      <c r="I28" s="98"/>
+      <c r="J28" s="98"/>
+      <c r="K28" s="98"/>
+      <c r="L28" s="98"/>
+      <c r="M28" s="98"/>
+      <c r="N28" s="98"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="94"/>
-      <c r="B29" s="94"/>
-      <c r="C29" s="94"/>
-      <c r="D29" s="94"/>
-      <c r="E29" s="94"/>
-      <c r="F29" s="94"/>
-      <c r="G29" s="94"/>
-      <c r="H29" s="94"/>
-      <c r="I29" s="94"/>
-      <c r="J29" s="94"/>
-      <c r="K29" s="94"/>
-      <c r="L29" s="94"/>
-      <c r="M29" s="94"/>
-      <c r="N29" s="94"/>
+      <c r="A29" s="98"/>
+      <c r="B29" s="98"/>
+      <c r="C29" s="98"/>
+      <c r="D29" s="98"/>
+      <c r="E29" s="98"/>
+      <c r="F29" s="98"/>
+      <c r="G29" s="98"/>
+      <c r="H29" s="98"/>
+      <c r="I29" s="98"/>
+      <c r="J29" s="98"/>
+      <c r="K29" s="98"/>
+      <c r="L29" s="98"/>
+      <c r="M29" s="98"/>
+      <c r="N29" s="98"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="94"/>
-      <c r="B30" s="94"/>
-      <c r="C30" s="94"/>
-      <c r="D30" s="94"/>
-      <c r="E30" s="94"/>
-      <c r="F30" s="94"/>
-      <c r="G30" s="94"/>
-      <c r="H30" s="94"/>
-      <c r="I30" s="94"/>
-      <c r="J30" s="94"/>
-      <c r="K30" s="94"/>
-      <c r="L30" s="94"/>
-      <c r="M30" s="94"/>
-      <c r="N30" s="94"/>
+      <c r="A30" s="98"/>
+      <c r="B30" s="98"/>
+      <c r="C30" s="98"/>
+      <c r="D30" s="98"/>
+      <c r="E30" s="98"/>
+      <c r="F30" s="98"/>
+      <c r="G30" s="98"/>
+      <c r="H30" s="98"/>
+      <c r="I30" s="98"/>
+      <c r="J30" s="98"/>
+      <c r="K30" s="98"/>
+      <c r="L30" s="98"/>
+      <c r="M30" s="98"/>
+      <c r="N30" s="98"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="94"/>
-      <c r="B31" s="94"/>
-      <c r="C31" s="94"/>
-      <c r="D31" s="94"/>
-      <c r="E31" s="94"/>
-      <c r="F31" s="94"/>
-      <c r="G31" s="94"/>
-      <c r="H31" s="94"/>
-      <c r="I31" s="94"/>
-      <c r="J31" s="94"/>
-      <c r="K31" s="94"/>
-      <c r="L31" s="94"/>
-      <c r="M31" s="94"/>
-      <c r="N31" s="94"/>
+      <c r="A31" s="98"/>
+      <c r="B31" s="98"/>
+      <c r="C31" s="98"/>
+      <c r="D31" s="98"/>
+      <c r="E31" s="98"/>
+      <c r="F31" s="98"/>
+      <c r="G31" s="98"/>
+      <c r="H31" s="98"/>
+      <c r="I31" s="98"/>
+      <c r="J31" s="98"/>
+      <c r="K31" s="98"/>
+      <c r="L31" s="98"/>
+      <c r="M31" s="98"/>
+      <c r="N31" s="98"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="94"/>
-      <c r="B32" s="94"/>
-      <c r="C32" s="94"/>
-      <c r="D32" s="94"/>
-      <c r="E32" s="94"/>
-      <c r="F32" s="94"/>
-      <c r="G32" s="94"/>
-      <c r="H32" s="94"/>
-      <c r="I32" s="94"/>
-      <c r="J32" s="94"/>
-      <c r="K32" s="94"/>
-      <c r="L32" s="94"/>
-      <c r="M32" s="94"/>
-      <c r="N32" s="94"/>
+      <c r="A32" s="98"/>
+      <c r="B32" s="98"/>
+      <c r="C32" s="98"/>
+      <c r="D32" s="98"/>
+      <c r="E32" s="98"/>
+      <c r="F32" s="98"/>
+      <c r="G32" s="98"/>
+      <c r="H32" s="98"/>
+      <c r="I32" s="98"/>
+      <c r="J32" s="98"/>
+      <c r="K32" s="98"/>
+      <c r="L32" s="98"/>
+      <c r="M32" s="98"/>
+      <c r="N32" s="98"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="94"/>
-      <c r="B33" s="94"/>
-      <c r="C33" s="94"/>
-      <c r="D33" s="94"/>
-      <c r="E33" s="94"/>
-      <c r="F33" s="94"/>
-      <c r="G33" s="94"/>
-      <c r="H33" s="94"/>
-      <c r="I33" s="94"/>
-      <c r="J33" s="94"/>
-      <c r="K33" s="94"/>
-      <c r="L33" s="94"/>
-      <c r="M33" s="94"/>
-      <c r="N33" s="94"/>
+      <c r="A33" s="98"/>
+      <c r="B33" s="98"/>
+      <c r="C33" s="98"/>
+      <c r="D33" s="98"/>
+      <c r="E33" s="98"/>
+      <c r="F33" s="98"/>
+      <c r="G33" s="98"/>
+      <c r="H33" s="98"/>
+      <c r="I33" s="98"/>
+      <c r="J33" s="98"/>
+      <c r="K33" s="98"/>
+      <c r="L33" s="98"/>
+      <c r="M33" s="98"/>
+      <c r="N33" s="98"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="94"/>
-      <c r="B34" s="94"/>
-      <c r="C34" s="94"/>
-      <c r="D34" s="94"/>
-      <c r="E34" s="94"/>
-      <c r="F34" s="94"/>
-      <c r="G34" s="94"/>
-      <c r="H34" s="94"/>
-      <c r="I34" s="94"/>
-      <c r="J34" s="94"/>
-      <c r="K34" s="94"/>
-      <c r="L34" s="94"/>
-      <c r="M34" s="94"/>
-      <c r="N34" s="94"/>
-      <c r="Q34" s="31"/>
+      <c r="A34" s="98"/>
+      <c r="B34" s="98"/>
+      <c r="C34" s="98"/>
+      <c r="D34" s="98"/>
+      <c r="E34" s="98"/>
+      <c r="F34" s="98"/>
+      <c r="G34" s="98"/>
+      <c r="H34" s="98"/>
+      <c r="I34" s="98"/>
+      <c r="J34" s="98"/>
+      <c r="K34" s="98"/>
+      <c r="L34" s="98"/>
+      <c r="M34" s="98"/>
+      <c r="N34" s="98"/>
+      <c r="Q34" s="30"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="94"/>
-      <c r="B35" s="94"/>
-      <c r="C35" s="94"/>
-      <c r="D35" s="94"/>
-      <c r="E35" s="94"/>
-      <c r="F35" s="94"/>
-      <c r="G35" s="94"/>
-      <c r="H35" s="94"/>
-      <c r="I35" s="94"/>
-      <c r="J35" s="94"/>
-      <c r="K35" s="94"/>
-      <c r="L35" s="94"/>
-      <c r="M35" s="94"/>
-      <c r="N35" s="94"/>
+      <c r="A35" s="98"/>
+      <c r="B35" s="98"/>
+      <c r="C35" s="98"/>
+      <c r="D35" s="98"/>
+      <c r="E35" s="98"/>
+      <c r="F35" s="98"/>
+      <c r="G35" s="98"/>
+      <c r="H35" s="98"/>
+      <c r="I35" s="98"/>
+      <c r="J35" s="98"/>
+      <c r="K35" s="98"/>
+      <c r="L35" s="98"/>
+      <c r="M35" s="98"/>
+      <c r="N35" s="98"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="94"/>
-      <c r="B36" s="94"/>
-      <c r="C36" s="94"/>
-      <c r="D36" s="94"/>
-      <c r="E36" s="94"/>
-      <c r="F36" s="94"/>
-      <c r="G36" s="94"/>
-      <c r="H36" s="94"/>
-      <c r="I36" s="94"/>
-      <c r="J36" s="94"/>
-      <c r="K36" s="94"/>
-      <c r="L36" s="94"/>
-      <c r="M36" s="94"/>
-      <c r="N36" s="94"/>
+      <c r="A36" s="98"/>
+      <c r="B36" s="98"/>
+      <c r="C36" s="98"/>
+      <c r="D36" s="98"/>
+      <c r="E36" s="98"/>
+      <c r="F36" s="98"/>
+      <c r="G36" s="98"/>
+      <c r="H36" s="98"/>
+      <c r="I36" s="98"/>
+      <c r="J36" s="98"/>
+      <c r="K36" s="98"/>
+      <c r="L36" s="98"/>
+      <c r="M36" s="98"/>
+      <c r="N36" s="98"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="94"/>
-      <c r="B37" s="94"/>
-      <c r="C37" s="94"/>
-      <c r="D37" s="94"/>
-      <c r="E37" s="94"/>
-      <c r="F37" s="94"/>
-      <c r="G37" s="94"/>
-      <c r="H37" s="94"/>
-      <c r="I37" s="94"/>
-      <c r="J37" s="94"/>
-      <c r="K37" s="94"/>
-      <c r="L37" s="94"/>
-      <c r="M37" s="94"/>
-      <c r="N37" s="94"/>
+      <c r="A37" s="98"/>
+      <c r="B37" s="98"/>
+      <c r="C37" s="98"/>
+      <c r="D37" s="98"/>
+      <c r="E37" s="98"/>
+      <c r="F37" s="98"/>
+      <c r="G37" s="98"/>
+      <c r="H37" s="98"/>
+      <c r="I37" s="98"/>
+      <c r="J37" s="98"/>
+      <c r="K37" s="98"/>
+      <c r="L37" s="98"/>
+      <c r="M37" s="98"/>
+      <c r="N37" s="98"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A38" s="94"/>
-      <c r="B38" s="94"/>
-      <c r="C38" s="94"/>
-      <c r="D38" s="94"/>
-      <c r="E38" s="94"/>
-      <c r="F38" s="94"/>
-      <c r="G38" s="94"/>
-      <c r="H38" s="94"/>
-      <c r="I38" s="94"/>
-      <c r="J38" s="94"/>
-      <c r="K38" s="94"/>
-      <c r="L38" s="94"/>
-      <c r="M38" s="94"/>
-      <c r="N38" s="94"/>
+      <c r="A38" s="98"/>
+      <c r="B38" s="98"/>
+      <c r="C38" s="98"/>
+      <c r="D38" s="98"/>
+      <c r="E38" s="98"/>
+      <c r="F38" s="98"/>
+      <c r="G38" s="98"/>
+      <c r="H38" s="98"/>
+      <c r="I38" s="98"/>
+      <c r="J38" s="98"/>
+      <c r="K38" s="98"/>
+      <c r="L38" s="98"/>
+      <c r="M38" s="98"/>
+      <c r="N38" s="98"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="94"/>
-      <c r="B39" s="94"/>
-      <c r="C39" s="94"/>
-      <c r="D39" s="94"/>
-      <c r="E39" s="94"/>
-      <c r="F39" s="94"/>
-      <c r="G39" s="94"/>
-      <c r="H39" s="94"/>
-      <c r="I39" s="94"/>
-      <c r="J39" s="94"/>
-      <c r="K39" s="94"/>
-      <c r="L39" s="94"/>
-      <c r="M39" s="94"/>
-      <c r="N39" s="94"/>
+      <c r="A39" s="98"/>
+      <c r="B39" s="98"/>
+      <c r="C39" s="98"/>
+      <c r="D39" s="98"/>
+      <c r="E39" s="98"/>
+      <c r="F39" s="98"/>
+      <c r="G39" s="98"/>
+      <c r="H39" s="98"/>
+      <c r="I39" s="98"/>
+      <c r="J39" s="98"/>
+      <c r="K39" s="98"/>
+      <c r="L39" s="98"/>
+      <c r="M39" s="98"/>
+      <c r="N39" s="98"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="94"/>
-      <c r="B40" s="94"/>
-      <c r="C40" s="94"/>
-      <c r="D40" s="94"/>
-      <c r="E40" s="94"/>
-      <c r="F40" s="94"/>
-      <c r="G40" s="94"/>
-      <c r="H40" s="94"/>
-      <c r="I40" s="94"/>
-      <c r="J40" s="94"/>
-      <c r="K40" s="94"/>
-      <c r="L40" s="94"/>
-      <c r="M40" s="94"/>
-      <c r="N40" s="94"/>
+      <c r="A40" s="98"/>
+      <c r="B40" s="98"/>
+      <c r="C40" s="98"/>
+      <c r="D40" s="98"/>
+      <c r="E40" s="98"/>
+      <c r="F40" s="98"/>
+      <c r="G40" s="98"/>
+      <c r="H40" s="98"/>
+      <c r="I40" s="98"/>
+      <c r="J40" s="98"/>
+      <c r="K40" s="98"/>
+      <c r="L40" s="98"/>
+      <c r="M40" s="98"/>
+      <c r="N40" s="98"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="94"/>
-      <c r="B41" s="94"/>
-      <c r="C41" s="94"/>
-      <c r="D41" s="94"/>
-      <c r="E41" s="94"/>
-      <c r="F41" s="94"/>
-      <c r="G41" s="94"/>
-      <c r="H41" s="94"/>
-      <c r="I41" s="94"/>
-      <c r="J41" s="94"/>
-      <c r="K41" s="94"/>
-      <c r="L41" s="94"/>
-      <c r="M41" s="94"/>
-      <c r="N41" s="94"/>
+      <c r="A41" s="98"/>
+      <c r="B41" s="98"/>
+      <c r="C41" s="98"/>
+      <c r="D41" s="98"/>
+      <c r="E41" s="98"/>
+      <c r="F41" s="98"/>
+      <c r="G41" s="98"/>
+      <c r="H41" s="98"/>
+      <c r="I41" s="98"/>
+      <c r="J41" s="98"/>
+      <c r="K41" s="98"/>
+      <c r="L41" s="98"/>
+      <c r="M41" s="98"/>
+      <c r="N41" s="98"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" s="94"/>
-      <c r="B42" s="94"/>
-      <c r="C42" s="94"/>
-      <c r="D42" s="94"/>
-      <c r="E42" s="94"/>
-      <c r="F42" s="94"/>
-      <c r="G42" s="94"/>
-      <c r="H42" s="94"/>
-      <c r="I42" s="94"/>
-      <c r="J42" s="94"/>
-      <c r="K42" s="94"/>
-      <c r="L42" s="94"/>
-      <c r="M42" s="94"/>
-      <c r="N42" s="94"/>
+      <c r="A42" s="98"/>
+      <c r="B42" s="98"/>
+      <c r="C42" s="98"/>
+      <c r="D42" s="98"/>
+      <c r="E42" s="98"/>
+      <c r="F42" s="98"/>
+      <c r="G42" s="98"/>
+      <c r="H42" s="98"/>
+      <c r="I42" s="98"/>
+      <c r="J42" s="98"/>
+      <c r="K42" s="98"/>
+      <c r="L42" s="98"/>
+      <c r="M42" s="98"/>
+      <c r="N42" s="98"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="94"/>
-      <c r="B43" s="94"/>
-      <c r="C43" s="94"/>
-      <c r="D43" s="94"/>
-      <c r="E43" s="94"/>
-      <c r="F43" s="94"/>
-      <c r="G43" s="94"/>
-      <c r="H43" s="94"/>
-      <c r="I43" s="94"/>
-      <c r="J43" s="94"/>
-      <c r="K43" s="94"/>
-      <c r="L43" s="94"/>
-      <c r="M43" s="94"/>
-      <c r="N43" s="94"/>
+      <c r="A43" s="98"/>
+      <c r="B43" s="98"/>
+      <c r="C43" s="98"/>
+      <c r="D43" s="98"/>
+      <c r="E43" s="98"/>
+      <c r="F43" s="98"/>
+      <c r="G43" s="98"/>
+      <c r="H43" s="98"/>
+      <c r="I43" s="98"/>
+      <c r="J43" s="98"/>
+      <c r="K43" s="98"/>
+      <c r="L43" s="98"/>
+      <c r="M43" s="98"/>
+      <c r="N43" s="98"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="94"/>
-      <c r="B44" s="94"/>
-      <c r="C44" s="94"/>
-      <c r="D44" s="94"/>
-      <c r="E44" s="94"/>
-      <c r="F44" s="94"/>
-      <c r="G44" s="94"/>
-      <c r="H44" s="94"/>
-      <c r="I44" s="94"/>
-      <c r="J44" s="94"/>
-      <c r="K44" s="94"/>
-      <c r="L44" s="94"/>
-      <c r="M44" s="94"/>
-      <c r="N44" s="94"/>
+      <c r="A44" s="98"/>
+      <c r="B44" s="98"/>
+      <c r="C44" s="98"/>
+      <c r="D44" s="98"/>
+      <c r="E44" s="98"/>
+      <c r="F44" s="98"/>
+      <c r="G44" s="98"/>
+      <c r="H44" s="98"/>
+      <c r="I44" s="98"/>
+      <c r="J44" s="98"/>
+      <c r="K44" s="98"/>
+      <c r="L44" s="98"/>
+      <c r="M44" s="98"/>
+      <c r="N44" s="98"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A45" s="94"/>
-      <c r="B45" s="94"/>
-      <c r="C45" s="94"/>
-      <c r="D45" s="94"/>
-      <c r="E45" s="94"/>
-      <c r="F45" s="94"/>
-      <c r="G45" s="94"/>
-      <c r="H45" s="94"/>
-      <c r="I45" s="94"/>
-      <c r="J45" s="94"/>
-      <c r="K45" s="94"/>
-      <c r="L45" s="94"/>
-      <c r="M45" s="94"/>
-      <c r="N45" s="94"/>
+      <c r="A45" s="98"/>
+      <c r="B45" s="98"/>
+      <c r="C45" s="98"/>
+      <c r="D45" s="98"/>
+      <c r="E45" s="98"/>
+      <c r="F45" s="98"/>
+      <c r="G45" s="98"/>
+      <c r="H45" s="98"/>
+      <c r="I45" s="98"/>
+      <c r="J45" s="98"/>
+      <c r="K45" s="98"/>
+      <c r="L45" s="98"/>
+      <c r="M45" s="98"/>
+      <c r="N45" s="98"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" s="94"/>
-      <c r="B46" s="94"/>
-      <c r="C46" s="94"/>
-      <c r="D46" s="94"/>
-      <c r="E46" s="94"/>
-      <c r="F46" s="94"/>
-      <c r="G46" s="94"/>
-      <c r="H46" s="94"/>
-      <c r="I46" s="94"/>
-      <c r="J46" s="94"/>
-      <c r="K46" s="94"/>
-      <c r="L46" s="94"/>
-      <c r="M46" s="94"/>
-      <c r="N46" s="94"/>
+      <c r="A46" s="98"/>
+      <c r="B46" s="98"/>
+      <c r="C46" s="98"/>
+      <c r="D46" s="98"/>
+      <c r="E46" s="98"/>
+      <c r="F46" s="98"/>
+      <c r="G46" s="98"/>
+      <c r="H46" s="98"/>
+      <c r="I46" s="98"/>
+      <c r="J46" s="98"/>
+      <c r="K46" s="98"/>
+      <c r="L46" s="98"/>
+      <c r="M46" s="98"/>
+      <c r="N46" s="98"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="94"/>
-      <c r="B47" s="94"/>
-      <c r="C47" s="94"/>
-      <c r="D47" s="94"/>
-      <c r="E47" s="94"/>
-      <c r="F47" s="94"/>
-      <c r="G47" s="94"/>
-      <c r="H47" s="94"/>
-      <c r="I47" s="94"/>
-      <c r="J47" s="94"/>
-      <c r="K47" s="94"/>
-      <c r="L47" s="94"/>
-      <c r="M47" s="94"/>
-      <c r="N47" s="94"/>
+      <c r="A47" s="98"/>
+      <c r="B47" s="98"/>
+      <c r="C47" s="98"/>
+      <c r="D47" s="98"/>
+      <c r="E47" s="98"/>
+      <c r="F47" s="98"/>
+      <c r="G47" s="98"/>
+      <c r="H47" s="98"/>
+      <c r="I47" s="98"/>
+      <c r="J47" s="98"/>
+      <c r="K47" s="98"/>
+      <c r="L47" s="98"/>
+      <c r="M47" s="98"/>
+      <c r="N47" s="98"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="94"/>
-      <c r="B48" s="94"/>
-      <c r="C48" s="94"/>
-      <c r="D48" s="94"/>
-      <c r="E48" s="94"/>
-      <c r="F48" s="94"/>
-      <c r="G48" s="94"/>
-      <c r="H48" s="94"/>
-      <c r="I48" s="94"/>
-      <c r="J48" s="94"/>
-      <c r="K48" s="94"/>
-      <c r="L48" s="94"/>
-      <c r="M48" s="94"/>
-      <c r="N48" s="94"/>
+      <c r="A48" s="98"/>
+      <c r="B48" s="98"/>
+      <c r="C48" s="98"/>
+      <c r="D48" s="98"/>
+      <c r="E48" s="98"/>
+      <c r="F48" s="98"/>
+      <c r="G48" s="98"/>
+      <c r="H48" s="98"/>
+      <c r="I48" s="98"/>
+      <c r="J48" s="98"/>
+      <c r="K48" s="98"/>
+      <c r="L48" s="98"/>
+      <c r="M48" s="98"/>
+      <c r="N48" s="98"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="lLBaIQOMgxT4Y8wf8AOw+JjKzMsMUmCIOvGewLOrNgNQrfdd02nwmes8yOvX5z1ZD2ZOe2ke60ralc025wUtNw==" saltValue="ubaVp5ncwgSQHgd+/t9/EA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="2nAGSGzWpWri71Pz9b2zCoiimyY7GVE3kRk9ZcsNGuTMBofv+KdGpUy/XwjTI75tE95Hz5k/eSFnJaGybVgrgQ==" saltValue="0Z7irvGJCQpnUu40SoDXjA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="B1 D1" name="Range1_28"/>
     <protectedRange sqref="C14:N14 C7:D8 F7:G8 F10:G13 I7:J8 I10:J13 L7:M8 L10:M13 C10:D13 C16:D16 F16:G16 I16:J16 L16:M16" name="Range1_28_1"/>
@@ -6389,6 +6401,15 @@
     <protectedRange sqref="L6:M6 C6:D6 F6:G6 I6:J6" name="Range1_28_1_3"/>
   </protectedRanges>
   <mergeCells count="20">
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A28:N48"/>
+    <mergeCell ref="A19:N19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="A2:A5"/>
@@ -6400,15 +6421,6 @@
     <mergeCell ref="I3:K4"/>
     <mergeCell ref="C2:K2"/>
     <mergeCell ref="L2:N2"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A28:N48"/>
-    <mergeCell ref="A19:N19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
   </mergeCells>
   <conditionalFormatting sqref="E10:E16 E6:E8">
     <cfRule type="cellIs" dxfId="44" priority="71" operator="equal">

</xml_diff>